<commit_message>
Se agrega CU EM-Profesor-CU1.3
</commit_message>
<xml_diff>
--- a/Documentacion Tecnica/PlaneacionCU/Planeacion.xlsx
+++ b/Documentacion Tecnica/PlaneacionCU/Planeacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8.1\Desktop\TT2\Documentacion\Documentacion Tecnica\PlaneacionCU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8.1\Desktop\ESCOMobile TT2\ESCOMobile\Documentacion Tecnica\PlaneacionCU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED33A544-546E-443C-A938-5D3581F39967}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA4D15B-701E-469D-9180-C8E6865B0D48}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{6BEE2BBB-66B6-49FE-B5FF-8E26273E1384}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="1" xr2:uid="{6BEE2BBB-66B6-49FE-B5FF-8E26273E1384}"/>
   </bookViews>
   <sheets>
     <sheet name="Planeación por módulos" sheetId="1" r:id="rId1"/>
@@ -536,7 +536,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="79">
+  <borders count="78">
     <border>
       <left/>
       <right/>
@@ -922,21 +922,6 @@
       </left>
       <right style="thin">
         <color theme="9" tint="-0.249977111117893"/>
-      </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="9" tint="-0.249977111117893"/>
-      </left>
-      <right style="medium">
-        <color theme="1"/>
       </right>
       <top style="medium">
         <color theme="1"/>
@@ -1589,129 +1574,126 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="59" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="65" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="66" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="72" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="73" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="64" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="65" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="71" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="72" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="73" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="76" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="76" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="77" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="76" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="77" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="76" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="77" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="78" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="78" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1727,12 +1709,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1742,15 +1745,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1760,17 +1754,32 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1781,19 +1790,19 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1802,25 +1811,25 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1829,63 +1838,37 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="71" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="71" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2202,8 +2185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9913E36-BDE9-470A-AFF3-2C8FCCD03D79}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B22"/>
+    <sheetView topLeftCell="B26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2219,15 +2202,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2253,10 +2236,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="99">
+      <c r="B3" s="94">
         <v>6</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -2268,16 +2251,16 @@
       <c r="E3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="89" t="s">
+      <c r="F3" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="88" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="106"/>
-      <c r="B4" s="101"/>
+      <c r="A4" s="97"/>
+      <c r="B4" s="99"/>
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
@@ -2287,16 +2270,16 @@
       <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="78" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="90" t="s">
+      <c r="F4" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="89" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="106"/>
-      <c r="B5" s="101"/>
+      <c r="A5" s="97"/>
+      <c r="B5" s="99"/>
       <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
@@ -2306,16 +2289,16 @@
       <c r="E5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="90" t="s">
+      <c r="F5" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="89" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="106"/>
-      <c r="B6" s="101"/>
+      <c r="A6" s="97"/>
+      <c r="B6" s="99"/>
       <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
@@ -2325,16 +2308,16 @@
       <c r="E6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="80" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="90" t="s">
+      <c r="F6" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="89" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="106"/>
-      <c r="B7" s="101"/>
+      <c r="A7" s="97"/>
+      <c r="B7" s="99"/>
       <c r="C7" s="27" t="s">
         <v>11</v>
       </c>
@@ -2344,16 +2327,16 @@
       <c r="E7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="90" t="s">
+      <c r="F7" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="89" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="107"/>
-      <c r="B8" s="100"/>
+      <c r="A8" s="98"/>
+      <c r="B8" s="95"/>
       <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
@@ -2363,19 +2346,19 @@
       <c r="E8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="85" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="91" t="s">
+      <c r="F8" s="84" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="90" t="s">
         <v>114</v>
       </c>
-      <c r="H8" s="92"/>
+      <c r="H8" s="91"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="99">
+      <c r="B9" s="94">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2387,16 +2370,16 @@
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="81" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="89" t="s">
+      <c r="F9" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="88" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="95"/>
-      <c r="B10" s="100"/>
+      <c r="A10" s="93"/>
+      <c r="B10" s="95"/>
       <c r="C10" s="18" t="s">
         <v>24</v>
       </c>
@@ -2406,18 +2389,18 @@
       <c r="E10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="82" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="91" t="s">
+      <c r="F10" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="90" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="99">
+      <c r="B11" s="94">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2429,16 +2412,16 @@
       <c r="E11" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="83" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="89" t="s">
+      <c r="F11" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="88" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="95"/>
-      <c r="B12" s="100"/>
+      <c r="A12" s="93"/>
+      <c r="B12" s="95"/>
       <c r="C12" s="18" t="s">
         <v>104</v>
       </c>
@@ -2448,18 +2431,18 @@
       <c r="E12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="84" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="91" t="s">
+      <c r="F12" s="83" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="90" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="99">
+      <c r="B13" s="94">
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2471,16 +2454,16 @@
       <c r="E13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="81" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="89" t="s">
+      <c r="F13" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="88" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="95"/>
-      <c r="B14" s="100"/>
+      <c r="A14" s="93"/>
+      <c r="B14" s="95"/>
       <c r="C14" s="18" t="s">
         <v>80</v>
       </c>
@@ -2490,18 +2473,18 @@
       <c r="E14" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="82" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="91" t="s">
+      <c r="F14" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="90" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="93" t="s">
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="99">
+      <c r="B15" s="94">
         <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2513,16 +2496,16 @@
       <c r="E15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="81" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="89" t="s">
+      <c r="F15" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="88" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="94"/>
-      <c r="B16" s="101"/>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="101"/>
+      <c r="B16" s="99"/>
       <c r="C16" s="12" t="s">
         <v>30</v>
       </c>
@@ -2532,16 +2515,16 @@
       <c r="E16" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="90" t="s">
+      <c r="F16" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="89" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="94"/>
-      <c r="B17" s="101"/>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="101"/>
+      <c r="B17" s="99"/>
       <c r="C17" s="3" t="s">
         <v>32</v>
       </c>
@@ -2552,15 +2535,15 @@
         <v>9</v>
       </c>
       <c r="F17" s="80" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="89" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="94"/>
-      <c r="B18" s="101"/>
+      <c r="A18" s="101"/>
+      <c r="B18" s="99"/>
       <c r="C18" s="12" t="s">
         <v>34</v>
       </c>
@@ -2570,16 +2553,16 @@
       <c r="E18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="90" t="s">
+      <c r="F18" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="89" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="94"/>
-      <c r="B19" s="101"/>
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="26" t="s">
         <v>36</v>
       </c>
@@ -2589,16 +2572,16 @@
       <c r="E19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="90" t="s">
+      <c r="F19" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="89" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="94"/>
-      <c r="B20" s="101"/>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="101"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="3" t="s">
         <v>101</v>
       </c>
@@ -2608,16 +2591,16 @@
       <c r="E20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="90" t="s">
+      <c r="F20" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="89" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="94"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="101"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="12" t="s">
         <v>38</v>
       </c>
@@ -2627,16 +2610,16 @@
       <c r="E21" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="90" t="s">
+      <c r="F21" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="89" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="95"/>
-      <c r="B22" s="100"/>
+      <c r="A22" s="93"/>
+      <c r="B22" s="95"/>
       <c r="C22" s="5" t="s">
         <v>32</v>
       </c>
@@ -2646,18 +2629,18 @@
       <c r="E22" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="85" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="91" t="s">
+      <c r="F22" s="84" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="90" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="102" t="s">
+      <c r="A23" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="96">
+      <c r="B23" s="102">
         <v>6</v>
       </c>
       <c r="C23" s="15" t="s">
@@ -2669,16 +2652,16 @@
       <c r="E23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="86" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="89" t="s">
+      <c r="F23" s="85" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="88" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="103"/>
-      <c r="B24" s="97"/>
+      <c r="A24" s="106"/>
+      <c r="B24" s="103"/>
       <c r="C24" s="3" t="s">
         <v>97</v>
       </c>
@@ -2688,10 +2671,10 @@
       <c r="E24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="80" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="90" t="s">
+      <c r="F24" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="89" t="s">
         <v>120</v>
       </c>
       <c r="H24" s="24"/>
@@ -2700,8 +2683,8 @@
       <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="103"/>
-      <c r="B25" s="97"/>
+      <c r="A25" s="106"/>
+      <c r="B25" s="103"/>
       <c r="C25" s="12" t="s">
         <v>98</v>
       </c>
@@ -2711,10 +2694,10 @@
       <c r="E25" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="90" t="s">
+      <c r="F25" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="89" t="s">
         <v>120</v>
       </c>
       <c r="H25" s="24"/>
@@ -2723,8 +2706,8 @@
       <c r="K25" s="24"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="103"/>
-      <c r="B26" s="97"/>
+      <c r="A26" s="106"/>
+      <c r="B26" s="103"/>
       <c r="C26" s="27" t="s">
         <v>102</v>
       </c>
@@ -2734,10 +2717,10 @@
       <c r="E26" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="90" t="s">
+      <c r="F26" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="89" t="s">
         <v>120</v>
       </c>
       <c r="H26" s="24"/>
@@ -2746,8 +2729,8 @@
       <c r="K26" s="24"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="103"/>
-      <c r="B27" s="97"/>
+      <c r="A27" s="106"/>
+      <c r="B27" s="103"/>
       <c r="C27" s="3" t="s">
         <v>99</v>
       </c>
@@ -2757,16 +2740,16 @@
       <c r="E27" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="90" t="s">
+      <c r="F27" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="89" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="104"/>
-      <c r="B28" s="98"/>
+      <c r="A28" s="107"/>
+      <c r="B28" s="104"/>
       <c r="C28" s="18" t="s">
         <v>46</v>
       </c>
@@ -2776,18 +2759,18 @@
       <c r="E28" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F28" s="84" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="91" t="s">
+      <c r="F28" s="83" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="90" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="102" t="s">
+      <c r="A29" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="99">
+      <c r="B29" s="94">
         <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -2799,16 +2782,16 @@
       <c r="E29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="83" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="89" t="s">
+      <c r="F29" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="88" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="103"/>
-      <c r="B30" s="101"/>
+      <c r="A30" s="106"/>
+      <c r="B30" s="99"/>
       <c r="C30" s="12" t="s">
         <v>53</v>
       </c>
@@ -2818,16 +2801,16 @@
       <c r="E30" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F30" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G30" s="90" t="s">
+      <c r="F30" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="89" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="103"/>
-      <c r="B31" s="101"/>
+      <c r="A31" s="106"/>
+      <c r="B31" s="99"/>
       <c r="C31" s="3" t="s">
         <v>55</v>
       </c>
@@ -2837,16 +2820,16 @@
       <c r="E31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="80" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="90" t="s">
+      <c r="F31" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="89" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="103"/>
-      <c r="B32" s="101"/>
+      <c r="A32" s="106"/>
+      <c r="B32" s="99"/>
       <c r="C32" s="12" t="s">
         <v>57</v>
       </c>
@@ -2856,16 +2839,16 @@
       <c r="E32" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F32" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="90" t="s">
+      <c r="F32" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="89" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="103"/>
-      <c r="B33" s="101"/>
+      <c r="A33" s="106"/>
+      <c r="B33" s="99"/>
       <c r="C33" s="3" t="s">
         <v>59</v>
       </c>
@@ -2875,16 +2858,16 @@
       <c r="E33" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="80" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="90" t="s">
+      <c r="F33" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="89" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="103"/>
-      <c r="B34" s="101"/>
+      <c r="A34" s="106"/>
+      <c r="B34" s="99"/>
       <c r="C34" s="12" t="s">
         <v>61</v>
       </c>
@@ -2894,16 +2877,16 @@
       <c r="E34" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F34" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="90" t="s">
+      <c r="F34" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="89" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="103"/>
-      <c r="B35" s="101"/>
+      <c r="A35" s="106"/>
+      <c r="B35" s="99"/>
       <c r="C35" s="3" t="s">
         <v>63</v>
       </c>
@@ -2913,16 +2896,16 @@
       <c r="E35" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="80" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="90" t="s">
+      <c r="F35" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="89" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="103"/>
-      <c r="B36" s="101"/>
+      <c r="A36" s="106"/>
+      <c r="B36" s="99"/>
       <c r="C36" s="12" t="s">
         <v>65</v>
       </c>
@@ -2932,16 +2915,16 @@
       <c r="E36" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="90" t="s">
+      <c r="F36" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="89" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="104"/>
-      <c r="B37" s="100"/>
+      <c r="A37" s="107"/>
+      <c r="B37" s="95"/>
       <c r="C37" s="5" t="s">
         <v>67</v>
       </c>
@@ -2951,18 +2934,18 @@
       <c r="E37" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F37" s="85" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="91" t="s">
+      <c r="F37" s="84" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="90" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="93" t="s">
+      <c r="A38" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="96">
+      <c r="B38" s="102">
         <v>10</v>
       </c>
       <c r="C38" s="15" t="s">
@@ -2974,16 +2957,16 @@
       <c r="E38" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" s="89" t="s">
+      <c r="F38" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="88" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="94"/>
-      <c r="B39" s="97"/>
+      <c r="A39" s="101"/>
+      <c r="B39" s="103"/>
       <c r="C39" s="3" t="s">
         <v>79</v>
       </c>
@@ -2993,16 +2976,16 @@
       <c r="E39" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F39" s="78" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="90" t="s">
+      <c r="F39" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="89" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="94"/>
-      <c r="B40" s="97"/>
+      <c r="A40" s="101"/>
+      <c r="B40" s="103"/>
       <c r="C40" s="12" t="s">
         <v>81</v>
       </c>
@@ -3012,16 +2995,16 @@
       <c r="E40" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F40" s="87" t="s">
-        <v>10</v>
-      </c>
-      <c r="G40" s="90" t="s">
+      <c r="F40" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="89" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="94"/>
-      <c r="B41" s="97"/>
+      <c r="A41" s="101"/>
+      <c r="B41" s="103"/>
       <c r="C41" s="3" t="s">
         <v>83</v>
       </c>
@@ -3031,16 +3014,16 @@
       <c r="E41" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F41" s="78" t="s">
-        <v>10</v>
-      </c>
-      <c r="G41" s="90" t="s">
+      <c r="F41" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="89" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="94"/>
-      <c r="B42" s="97"/>
+      <c r="A42" s="101"/>
+      <c r="B42" s="103"/>
       <c r="C42" s="12" t="s">
         <v>77</v>
       </c>
@@ -3050,16 +3033,16 @@
       <c r="E42" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F42" s="87" t="s">
-        <v>10</v>
-      </c>
-      <c r="G42" s="90" t="s">
+      <c r="F42" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="89" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="94"/>
-      <c r="B43" s="97"/>
+      <c r="A43" s="101"/>
+      <c r="B43" s="103"/>
       <c r="C43" s="3" t="s">
         <v>86</v>
       </c>
@@ -3069,16 +3052,16 @@
       <c r="E43" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="78" t="s">
-        <v>10</v>
-      </c>
-      <c r="G43" s="90" t="s">
+      <c r="F43" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="89" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="94"/>
-      <c r="B44" s="97"/>
+      <c r="A44" s="101"/>
+      <c r="B44" s="103"/>
       <c r="C44" s="12" t="s">
         <v>88</v>
       </c>
@@ -3088,16 +3071,16 @@
       <c r="E44" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F44" s="87" t="s">
-        <v>10</v>
-      </c>
-      <c r="G44" s="90" t="s">
+      <c r="F44" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="89" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="94"/>
-      <c r="B45" s="97"/>
+      <c r="A45" s="101"/>
+      <c r="B45" s="103"/>
       <c r="C45" s="3" t="s">
         <v>90</v>
       </c>
@@ -3107,16 +3090,16 @@
       <c r="E45" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F45" s="78" t="s">
-        <v>10</v>
-      </c>
-      <c r="G45" s="90" t="s">
+      <c r="F45" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="89" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="94"/>
-      <c r="B46" s="97"/>
+      <c r="A46" s="101"/>
+      <c r="B46" s="103"/>
       <c r="C46" s="12" t="s">
         <v>92</v>
       </c>
@@ -3126,16 +3109,16 @@
       <c r="E46" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F46" s="87" t="s">
-        <v>10</v>
-      </c>
-      <c r="G46" s="90" t="s">
+      <c r="F46" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" s="89" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="95"/>
-      <c r="B47" s="98"/>
+      <c r="A47" s="93"/>
+      <c r="B47" s="104"/>
       <c r="C47" s="5" t="s">
         <v>94</v>
       </c>
@@ -3145,20 +3128,15 @@
       <c r="E47" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F47" s="88" t="s">
-        <v>10</v>
-      </c>
-      <c r="G47" s="91" t="s">
+      <c r="F47" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="90" t="s">
         <v>121</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="A1:G1"/>
     <mergeCell ref="A38:A47"/>
     <mergeCell ref="B38:B47"/>
     <mergeCell ref="A13:A14"/>
@@ -3171,6 +3149,11 @@
     <mergeCell ref="B23:B28"/>
     <mergeCell ref="B29:B37"/>
     <mergeCell ref="A29:A37"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3181,8 +3164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8E41A5-F136-4AC2-820E-22508AAAA400}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3196,14 +3179,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="117" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
@@ -3226,10 +3209,10 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="113" t="s">
+      <c r="A3" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="110">
+      <c r="B3" s="118">
         <v>21</v>
       </c>
       <c r="C3" s="34" t="s">
@@ -3238,37 +3221,37 @@
       <c r="D3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="124" t="s">
+      <c r="E3" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="36" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="114"/>
-      <c r="B4" s="111"/>
+      <c r="A4" s="122"/>
+      <c r="B4" s="119"/>
       <c r="C4" s="30" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="125"/>
+      <c r="E4" s="133"/>
       <c r="F4" s="36" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="114"/>
-      <c r="B5" s="111"/>
+      <c r="A5" s="122"/>
+      <c r="B5" s="119"/>
       <c r="C5" s="30" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="126" t="s">
+      <c r="E5" s="134" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="36" t="s">
@@ -3276,29 +3259,29 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="114"/>
-      <c r="B6" s="111"/>
+      <c r="A6" s="122"/>
+      <c r="B6" s="119"/>
       <c r="C6" s="30" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="125"/>
+      <c r="E6" s="133"/>
       <c r="F6" s="36" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="114"/>
-      <c r="B7" s="111"/>
+      <c r="A7" s="122"/>
+      <c r="B7" s="119"/>
       <c r="C7" s="30" t="s">
         <v>71</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="126" t="s">
+      <c r="E7" s="134" t="s">
         <v>70</v>
       </c>
       <c r="F7" s="36" t="s">
@@ -3310,15 +3293,15 @@
       <c r="K7" s="24"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="114"/>
-      <c r="B8" s="111"/>
+      <c r="A8" s="122"/>
+      <c r="B8" s="119"/>
       <c r="C8" s="30" t="s">
         <v>80</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="125"/>
+      <c r="E8" s="133"/>
       <c r="F8" s="36" t="s">
         <v>10</v>
       </c>
@@ -3328,15 +3311,15 @@
       <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="114"/>
-      <c r="B9" s="111"/>
+      <c r="A9" s="122"/>
+      <c r="B9" s="119"/>
       <c r="C9" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="146" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="126" t="s">
+      <c r="E9" s="134" t="s">
         <v>27</v>
       </c>
       <c r="F9" s="36" t="s">
@@ -3348,15 +3331,15 @@
       <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="114"/>
-      <c r="B10" s="111"/>
+      <c r="A10" s="122"/>
+      <c r="B10" s="119"/>
       <c r="C10" s="30" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="127"/>
+      <c r="E10" s="135"/>
       <c r="F10" s="36" t="s">
         <v>16</v>
       </c>
@@ -3366,15 +3349,15 @@
       <c r="K10" s="24"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="114"/>
-      <c r="B11" s="111"/>
+      <c r="A11" s="122"/>
+      <c r="B11" s="119"/>
       <c r="C11" s="30" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="127"/>
+      <c r="E11" s="135"/>
       <c r="F11" s="36" t="s">
         <v>10</v>
       </c>
@@ -3384,15 +3367,15 @@
       <c r="K11" s="24"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="114"/>
-      <c r="B12" s="111"/>
+      <c r="A12" s="122"/>
+      <c r="B12" s="119"/>
       <c r="C12" s="30" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="127"/>
+      <c r="E12" s="135"/>
       <c r="F12" s="37" t="s">
         <v>16</v>
       </c>
@@ -3402,15 +3385,15 @@
       <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="114"/>
-      <c r="B13" s="111"/>
+      <c r="A13" s="122"/>
+      <c r="B13" s="119"/>
       <c r="C13" s="30" t="s">
         <v>101</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="127"/>
+      <c r="E13" s="135"/>
       <c r="F13" s="36" t="s">
         <v>10</v>
       </c>
@@ -3420,17 +3403,17 @@
       <c r="K13" s="24"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="114"/>
-      <c r="B14" s="111"/>
+      <c r="A14" s="122"/>
+      <c r="B14" s="119"/>
       <c r="C14" s="30" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="127"/>
-      <c r="F14" s="49" t="s">
-        <v>16</v>
+      <c r="E14" s="135"/>
+      <c r="F14" s="36" t="s">
+        <v>10</v>
       </c>
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
@@ -3438,15 +3421,15 @@
       <c r="K14" s="24"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="114"/>
-      <c r="B15" s="111"/>
+      <c r="A15" s="122"/>
+      <c r="B15" s="119"/>
       <c r="C15" s="30" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="125"/>
+      <c r="E15" s="133"/>
       <c r="F15" s="37" t="s">
         <v>16</v>
       </c>
@@ -3456,15 +3439,15 @@
       <c r="K15" s="24"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="114"/>
-      <c r="B16" s="111"/>
+      <c r="A16" s="122"/>
+      <c r="B16" s="119"/>
       <c r="C16" s="30" t="s">
         <v>51</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="126" t="s">
+      <c r="E16" s="134" t="s">
         <v>69</v>
       </c>
       <c r="F16" s="37" t="s">
@@ -3476,15 +3459,15 @@
       <c r="K16" s="24"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="114"/>
-      <c r="B17" s="111"/>
+      <c r="A17" s="122"/>
+      <c r="B17" s="119"/>
       <c r="C17" s="30" t="s">
         <v>55</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="127"/>
+      <c r="E17" s="135"/>
       <c r="F17" s="37" t="s">
         <v>16</v>
       </c>
@@ -3494,15 +3477,15 @@
       <c r="K17" s="24"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="114"/>
-      <c r="B18" s="111"/>
+      <c r="A18" s="122"/>
+      <c r="B18" s="119"/>
       <c r="C18" s="30" t="s">
         <v>65</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="125"/>
+      <c r="E18" s="133"/>
       <c r="F18" s="37" t="s">
         <v>16</v>
       </c>
@@ -3512,15 +3495,15 @@
       <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="114"/>
-      <c r="B19" s="111"/>
+      <c r="A19" s="122"/>
+      <c r="B19" s="119"/>
       <c r="C19" s="30" t="s">
         <v>75</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="126" t="s">
+      <c r="E19" s="134" t="s">
         <v>74</v>
       </c>
       <c r="F19" s="36" t="s">
@@ -3532,15 +3515,15 @@
       <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="114"/>
-      <c r="B20" s="111"/>
+      <c r="A20" s="122"/>
+      <c r="B20" s="119"/>
       <c r="C20" s="30" t="s">
         <v>79</v>
       </c>
       <c r="D20" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="127"/>
+      <c r="E20" s="135"/>
       <c r="F20" s="36" t="s">
         <v>10</v>
       </c>
@@ -3550,16 +3533,16 @@
       <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="114"/>
-      <c r="B21" s="111"/>
+      <c r="A21" s="122"/>
+      <c r="B21" s="119"/>
       <c r="C21" s="30" t="s">
         <v>86</v>
       </c>
       <c r="D21" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="127"/>
-      <c r="F21" s="49" t="s">
+      <c r="E21" s="135"/>
+      <c r="F21" s="48" t="s">
         <v>10</v>
       </c>
       <c r="H21" s="24"/>
@@ -3568,15 +3551,15 @@
       <c r="K21" s="24"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="114"/>
-      <c r="B22" s="111"/>
+      <c r="A22" s="122"/>
+      <c r="B22" s="119"/>
       <c r="C22" s="30" t="s">
         <v>88</v>
       </c>
       <c r="D22" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="127"/>
+      <c r="E22" s="135"/>
       <c r="F22" s="36" t="s">
         <v>10</v>
       </c>
@@ -3586,15 +3569,15 @@
       <c r="K22" s="24"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="115"/>
-      <c r="B23" s="112"/>
+      <c r="A23" s="123"/>
+      <c r="B23" s="120"/>
       <c r="C23" s="38" t="s">
         <v>90</v>
       </c>
       <c r="D23" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="128"/>
+      <c r="E23" s="136"/>
       <c r="F23" s="40" t="s">
         <v>10</v>
       </c>
@@ -3604,10 +3587,10 @@
       <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="119" t="s">
+      <c r="A24" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="116">
+      <c r="B24" s="124">
         <v>21</v>
       </c>
       <c r="C24" s="41" t="s">
@@ -3619,7 +3602,7 @@
       <c r="E24" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="64" t="s">
+      <c r="F24" s="63" t="s">
         <v>10</v>
       </c>
       <c r="H24" s="24"/>
@@ -3628,15 +3611,15 @@
       <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="120"/>
-      <c r="B25" s="117"/>
+      <c r="A25" s="128"/>
+      <c r="B25" s="125"/>
       <c r="C25" s="32" t="s">
         <v>43</v>
       </c>
       <c r="D25" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="E25" s="122" t="s">
+      <c r="E25" s="130" t="s">
         <v>42</v>
       </c>
       <c r="F25" s="43" t="s">
@@ -3648,15 +3631,15 @@
       <c r="K25" s="24"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="120"/>
-      <c r="B26" s="117"/>
+      <c r="A26" s="128"/>
+      <c r="B26" s="125"/>
       <c r="C26" s="32" t="s">
         <v>104</v>
       </c>
       <c r="D26" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="E26" s="129"/>
+      <c r="E26" s="137"/>
       <c r="F26" s="43" t="s">
         <v>16</v>
       </c>
@@ -3666,8 +3649,8 @@
       <c r="K26" s="24"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="120"/>
-      <c r="B27" s="117"/>
+      <c r="A27" s="128"/>
+      <c r="B27" s="125"/>
       <c r="C27" s="32" t="s">
         <v>34</v>
       </c>
@@ -3682,15 +3665,15 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="120"/>
-      <c r="B28" s="117"/>
+      <c r="A28" s="128"/>
+      <c r="B28" s="125"/>
       <c r="C28" s="32" t="s">
         <v>44</v>
       </c>
       <c r="D28" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="122" t="s">
+      <c r="E28" s="130" t="s">
         <v>108</v>
       </c>
       <c r="F28" s="43" t="s">
@@ -3698,85 +3681,85 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="120"/>
-      <c r="B29" s="117"/>
+      <c r="A29" s="128"/>
+      <c r="B29" s="125"/>
       <c r="C29" s="32" t="s">
         <v>97</v>
       </c>
       <c r="D29" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="123"/>
+      <c r="E29" s="131"/>
       <c r="F29" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="120"/>
-      <c r="B30" s="117"/>
+      <c r="A30" s="128"/>
+      <c r="B30" s="125"/>
       <c r="C30" s="32" t="s">
         <v>98</v>
       </c>
       <c r="D30" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="123"/>
+      <c r="E30" s="131"/>
       <c r="F30" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="120"/>
-      <c r="B31" s="117"/>
+      <c r="A31" s="128"/>
+      <c r="B31" s="125"/>
       <c r="C31" s="32" t="s">
         <v>102</v>
       </c>
       <c r="D31" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="E31" s="123"/>
+      <c r="E31" s="131"/>
       <c r="F31" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="120"/>
-      <c r="B32" s="117"/>
+      <c r="A32" s="128"/>
+      <c r="B32" s="125"/>
       <c r="C32" s="32" t="s">
         <v>99</v>
       </c>
       <c r="D32" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="123"/>
+      <c r="E32" s="131"/>
       <c r="F32" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="120"/>
-      <c r="B33" s="117"/>
+      <c r="A33" s="128"/>
+      <c r="B33" s="125"/>
       <c r="C33" s="32" t="s">
         <v>46</v>
       </c>
       <c r="D33" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="129"/>
+      <c r="E33" s="137"/>
       <c r="F33" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="120"/>
-      <c r="B34" s="117"/>
+      <c r="A34" s="128"/>
+      <c r="B34" s="125"/>
       <c r="C34" s="32" t="s">
         <v>53</v>
       </c>
       <c r="D34" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="122" t="s">
+      <c r="E34" s="130" t="s">
         <v>69</v>
       </c>
       <c r="F34" s="43" t="s">
@@ -3784,85 +3767,85 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="120"/>
-      <c r="B35" s="117"/>
+      <c r="A35" s="128"/>
+      <c r="B35" s="125"/>
       <c r="C35" s="32" t="s">
         <v>57</v>
       </c>
       <c r="D35" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="123"/>
+      <c r="E35" s="131"/>
       <c r="F35" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="120"/>
-      <c r="B36" s="117"/>
+      <c r="A36" s="128"/>
+      <c r="B36" s="125"/>
       <c r="C36" s="32" t="s">
         <v>59</v>
       </c>
       <c r="D36" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="123"/>
+      <c r="E36" s="131"/>
       <c r="F36" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="120"/>
-      <c r="B37" s="117"/>
+      <c r="A37" s="128"/>
+      <c r="B37" s="125"/>
       <c r="C37" s="32" t="s">
         <v>61</v>
       </c>
       <c r="D37" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="123"/>
+      <c r="E37" s="131"/>
       <c r="F37" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="120"/>
-      <c r="B38" s="117"/>
+      <c r="A38" s="128"/>
+      <c r="B38" s="125"/>
       <c r="C38" s="32" t="s">
         <v>63</v>
       </c>
       <c r="D38" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="E38" s="123"/>
+      <c r="E38" s="131"/>
       <c r="F38" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="120"/>
-      <c r="B39" s="117"/>
+      <c r="A39" s="128"/>
+      <c r="B39" s="125"/>
       <c r="C39" s="32" t="s">
         <v>67</v>
       </c>
       <c r="D39" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="E39" s="129"/>
+      <c r="E39" s="137"/>
       <c r="F39" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="120"/>
-      <c r="B40" s="117"/>
+      <c r="A40" s="128"/>
+      <c r="B40" s="125"/>
       <c r="C40" s="32" t="s">
         <v>81</v>
       </c>
       <c r="D40" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="E40" s="122" t="s">
+      <c r="E40" s="130" t="s">
         <v>74</v>
       </c>
       <c r="F40" s="43" t="s">
@@ -3872,112 +3855,114 @@
       <c r="H40" s="24"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="120"/>
-      <c r="B41" s="117"/>
+      <c r="A41" s="128"/>
+      <c r="B41" s="125"/>
       <c r="C41" s="32" t="s">
         <v>83</v>
       </c>
       <c r="D41" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="E41" s="123"/>
+      <c r="E41" s="131"/>
       <c r="F41" s="43" t="s">
         <v>10</v>
       </c>
       <c r="G41" s="45"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="120"/>
-      <c r="B42" s="117"/>
+      <c r="A42" s="128"/>
+      <c r="B42" s="125"/>
       <c r="C42" s="32" t="s">
         <v>77</v>
       </c>
       <c r="D42" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="E42" s="123"/>
+      <c r="E42" s="131"/>
       <c r="F42" s="44" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="120"/>
-      <c r="B43" s="117"/>
+      <c r="A43" s="128"/>
+      <c r="B43" s="125"/>
       <c r="C43" s="32" t="s">
         <v>92</v>
       </c>
       <c r="D43" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="E43" s="123"/>
+      <c r="E43" s="131"/>
       <c r="F43" s="43" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="121"/>
-      <c r="B44" s="118"/>
-      <c r="C44" s="67" t="s">
+      <c r="A44" s="129"/>
+      <c r="B44" s="126"/>
+      <c r="C44" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="68" t="s">
+      <c r="D44" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="E44" s="123"/>
-      <c r="F44" s="69" t="s">
+      <c r="E44" s="131"/>
+      <c r="F44" s="68" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="130" t="s">
+      <c r="A45" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="133">
+      <c r="B45" s="111">
         <v>2</v>
       </c>
-      <c r="C45" s="70" t="s">
+      <c r="C45" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="D45" s="71" t="s">
+      <c r="D45" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="E45" s="136" t="s">
+      <c r="E45" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="F45" s="72" t="s">
+      <c r="F45" s="71" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="131"/>
-      <c r="B46" s="134"/>
-      <c r="C46" s="65" t="s">
+      <c r="A46" s="109"/>
+      <c r="B46" s="112"/>
+      <c r="C46" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="66" t="s">
+      <c r="D46" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="E46" s="137"/>
-      <c r="F46" s="73" t="s">
+      <c r="E46" s="115"/>
+      <c r="F46" s="72" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="132"/>
-      <c r="B47" s="135"/>
-      <c r="C47" s="74" t="s">
+      <c r="A47" s="110"/>
+      <c r="B47" s="113"/>
+      <c r="C47" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="75" t="s">
+      <c r="D47" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="E47" s="138"/>
-      <c r="F47" s="76" t="s">
+      <c r="E47" s="116"/>
+      <c r="F47" s="75" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E5:E6"/>
     <mergeCell ref="A45:A47"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="E45:E47"/>
@@ -3994,10 +3979,9 @@
     <mergeCell ref="E28:E33"/>
     <mergeCell ref="E34:E39"/>
     <mergeCell ref="E9:E15"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4019,117 +4003,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="138" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="51" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="140" t="s">
+      <c r="A3" s="139" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="54" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="145" t="s">
+      <c r="D3" s="144" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="63" t="s">
+      <c r="E3" s="62" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="141"/>
+      <c r="A4" s="140"/>
       <c r="B4" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="145"/>
-      <c r="E4" s="62" t="s">
+      <c r="D4" s="144"/>
+      <c r="E4" s="61" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="141"/>
-      <c r="B5" s="56" t="s">
+      <c r="A5" s="140"/>
+      <c r="B5" s="55" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="145"/>
-      <c r="E5" s="61" t="s">
+      <c r="D5" s="144"/>
+      <c r="E5" s="60" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="141"/>
+      <c r="A6" s="140"/>
       <c r="B6" s="27" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="145"/>
-      <c r="E6" s="61" t="s">
+      <c r="D6" s="144"/>
+      <c r="E6" s="60" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="141"/>
-      <c r="B7" s="56" t="s">
+      <c r="A7" s="140"/>
+      <c r="B7" s="55" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="146"/>
-      <c r="E7" s="53" t="s">
+      <c r="D7" s="145"/>
+      <c r="E7" s="52" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="142"/>
+      <c r="A8" s="141"/>
       <c r="B8" s="27" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="60" t="s">
+      <c r="D8" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="58" t="s">
+      <c r="E8" s="57" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="143" t="s">
+      <c r="A9" s="142" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="27" t="s">
@@ -4138,25 +4122,25 @@
       <c r="C9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="61" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="144"/>
-      <c r="B10" s="57" t="s">
+      <c r="A10" s="143"/>
+      <c r="B10" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="E10" s="53" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se termina redacción de CU para módulo de Profesor
</commit_message>
<xml_diff>
--- a/Documentacion Tecnica/PlaneacionCU/Planeacion.xlsx
+++ b/Documentacion Tecnica/PlaneacionCU/Planeacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8.1\Desktop\ESCOMobile TT2\ESCOMobile\Documentacion Tecnica\PlaneacionCU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA4D15B-701E-469D-9180-C8E6865B0D48}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD66125-AFF0-42FC-B115-9C516B1BAADE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="1" xr2:uid="{6BEE2BBB-66B6-49FE-B5FF-8E26273E1384}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{6BEE2BBB-66B6-49FE-B5FF-8E26273E1384}"/>
   </bookViews>
   <sheets>
     <sheet name="Planeación por módulos" sheetId="1" r:id="rId1"/>
@@ -1706,18 +1706,43 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1727,32 +1752,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1829,12 +1836,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1868,7 +1869,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2185,8 +2185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9913E36-BDE9-470A-AFF3-2C8FCCD03D79}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView topLeftCell="B26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2202,15 +2202,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2236,10 +2236,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="94">
+      <c r="B3" s="99">
         <v>6</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -2259,8 +2259,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="97"/>
-      <c r="B4" s="99"/>
+      <c r="A4" s="106"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
@@ -2278,8 +2278,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="97"/>
-      <c r="B5" s="99"/>
+      <c r="A5" s="106"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
@@ -2297,8 +2297,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="97"/>
-      <c r="B6" s="99"/>
+      <c r="A6" s="106"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
@@ -2316,8 +2316,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="97"/>
-      <c r="B7" s="99"/>
+      <c r="A7" s="106"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="27" t="s">
         <v>11</v>
       </c>
@@ -2335,8 +2335,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="98"/>
-      <c r="B8" s="95"/>
+      <c r="A8" s="107"/>
+      <c r="B8" s="100"/>
       <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
@@ -2355,10 +2355,10 @@
       <c r="H8" s="91"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="92" t="s">
+      <c r="A9" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="94">
+      <c r="B9" s="99">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2378,8 +2378,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="93"/>
-      <c r="B10" s="95"/>
+      <c r="A10" s="95"/>
+      <c r="B10" s="100"/>
       <c r="C10" s="18" t="s">
         <v>24</v>
       </c>
@@ -2397,10 +2397,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="92" t="s">
+      <c r="A11" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="94">
+      <c r="B11" s="99">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2420,8 +2420,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="93"/>
-      <c r="B12" s="95"/>
+      <c r="A12" s="95"/>
+      <c r="B12" s="100"/>
       <c r="C12" s="18" t="s">
         <v>104</v>
       </c>
@@ -2439,10 +2439,10 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="92" t="s">
+      <c r="A13" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="94">
+      <c r="B13" s="99">
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2462,8 +2462,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="93"/>
-      <c r="B14" s="95"/>
+      <c r="A14" s="95"/>
+      <c r="B14" s="100"/>
       <c r="C14" s="18" t="s">
         <v>80</v>
       </c>
@@ -2481,10 +2481,10 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="92" t="s">
+      <c r="A15" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="94">
+      <c r="B15" s="99">
         <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2504,8 +2504,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="101"/>
-      <c r="B16" s="99"/>
+      <c r="A16" s="94"/>
+      <c r="B16" s="101"/>
       <c r="C16" s="12" t="s">
         <v>30</v>
       </c>
@@ -2523,8 +2523,8 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="101"/>
-      <c r="B17" s="99"/>
+      <c r="A17" s="94"/>
+      <c r="B17" s="101"/>
       <c r="C17" s="3" t="s">
         <v>32</v>
       </c>
@@ -2542,8 +2542,8 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="101"/>
-      <c r="B18" s="99"/>
+      <c r="A18" s="94"/>
+      <c r="B18" s="101"/>
       <c r="C18" s="12" t="s">
         <v>34</v>
       </c>
@@ -2561,8 +2561,8 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="101"/>
-      <c r="B19" s="99"/>
+      <c r="A19" s="94"/>
+      <c r="B19" s="101"/>
       <c r="C19" s="26" t="s">
         <v>36</v>
       </c>
@@ -2580,8 +2580,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="101"/>
-      <c r="B20" s="99"/>
+      <c r="A20" s="94"/>
+      <c r="B20" s="101"/>
       <c r="C20" s="3" t="s">
         <v>101</v>
       </c>
@@ -2599,8 +2599,8 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="101"/>
-      <c r="B21" s="99"/>
+      <c r="A21" s="94"/>
+      <c r="B21" s="101"/>
       <c r="C21" s="12" t="s">
         <v>38</v>
       </c>
@@ -2618,8 +2618,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="93"/>
-      <c r="B22" s="95"/>
+      <c r="A22" s="95"/>
+      <c r="B22" s="100"/>
       <c r="C22" s="5" t="s">
         <v>32</v>
       </c>
@@ -2637,10 +2637,10 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="105" t="s">
+      <c r="A23" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="102">
+      <c r="B23" s="96">
         <v>6</v>
       </c>
       <c r="C23" s="15" t="s">
@@ -2660,8 +2660,8 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="106"/>
-      <c r="B24" s="103"/>
+      <c r="A24" s="103"/>
+      <c r="B24" s="97"/>
       <c r="C24" s="3" t="s">
         <v>97</v>
       </c>
@@ -2683,8 +2683,8 @@
       <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="106"/>
-      <c r="B25" s="103"/>
+      <c r="A25" s="103"/>
+      <c r="B25" s="97"/>
       <c r="C25" s="12" t="s">
         <v>98</v>
       </c>
@@ -2706,8 +2706,8 @@
       <c r="K25" s="24"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="106"/>
-      <c r="B26" s="103"/>
+      <c r="A26" s="103"/>
+      <c r="B26" s="97"/>
       <c r="C26" s="27" t="s">
         <v>102</v>
       </c>
@@ -2729,8 +2729,8 @@
       <c r="K26" s="24"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="106"/>
-      <c r="B27" s="103"/>
+      <c r="A27" s="103"/>
+      <c r="B27" s="97"/>
       <c r="C27" s="3" t="s">
         <v>99</v>
       </c>
@@ -2748,8 +2748,8 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="107"/>
-      <c r="B28" s="104"/>
+      <c r="A28" s="104"/>
+      <c r="B28" s="98"/>
       <c r="C28" s="18" t="s">
         <v>46</v>
       </c>
@@ -2767,10 +2767,10 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="105" t="s">
+      <c r="A29" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="94">
+      <c r="B29" s="99">
         <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -2790,8 +2790,8 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="106"/>
-      <c r="B30" s="99"/>
+      <c r="A30" s="103"/>
+      <c r="B30" s="101"/>
       <c r="C30" s="12" t="s">
         <v>53</v>
       </c>
@@ -2809,8 +2809,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="106"/>
-      <c r="B31" s="99"/>
+      <c r="A31" s="103"/>
+      <c r="B31" s="101"/>
       <c r="C31" s="3" t="s">
         <v>55</v>
       </c>
@@ -2828,8 +2828,8 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="106"/>
-      <c r="B32" s="99"/>
+      <c r="A32" s="103"/>
+      <c r="B32" s="101"/>
       <c r="C32" s="12" t="s">
         <v>57</v>
       </c>
@@ -2847,8 +2847,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="106"/>
-      <c r="B33" s="99"/>
+      <c r="A33" s="103"/>
+      <c r="B33" s="101"/>
       <c r="C33" s="3" t="s">
         <v>59</v>
       </c>
@@ -2866,8 +2866,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="106"/>
-      <c r="B34" s="99"/>
+      <c r="A34" s="103"/>
+      <c r="B34" s="101"/>
       <c r="C34" s="12" t="s">
         <v>61</v>
       </c>
@@ -2885,8 +2885,8 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="106"/>
-      <c r="B35" s="99"/>
+      <c r="A35" s="103"/>
+      <c r="B35" s="101"/>
       <c r="C35" s="3" t="s">
         <v>63</v>
       </c>
@@ -2904,8 +2904,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="106"/>
-      <c r="B36" s="99"/>
+      <c r="A36" s="103"/>
+      <c r="B36" s="101"/>
       <c r="C36" s="12" t="s">
         <v>65</v>
       </c>
@@ -2923,8 +2923,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="107"/>
-      <c r="B37" s="95"/>
+      <c r="A37" s="104"/>
+      <c r="B37" s="100"/>
       <c r="C37" s="5" t="s">
         <v>67</v>
       </c>
@@ -2942,10 +2942,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="92" t="s">
+      <c r="A38" s="93" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="102">
+      <c r="B38" s="96">
         <v>10</v>
       </c>
       <c r="C38" s="15" t="s">
@@ -2965,8 +2965,8 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="101"/>
-      <c r="B39" s="103"/>
+      <c r="A39" s="94"/>
+      <c r="B39" s="97"/>
       <c r="C39" s="3" t="s">
         <v>79</v>
       </c>
@@ -2984,8 +2984,8 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="101"/>
-      <c r="B40" s="103"/>
+      <c r="A40" s="94"/>
+      <c r="B40" s="97"/>
       <c r="C40" s="12" t="s">
         <v>81</v>
       </c>
@@ -3003,8 +3003,8 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="101"/>
-      <c r="B41" s="103"/>
+      <c r="A41" s="94"/>
+      <c r="B41" s="97"/>
       <c r="C41" s="3" t="s">
         <v>83</v>
       </c>
@@ -3022,8 +3022,8 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="101"/>
-      <c r="B42" s="103"/>
+      <c r="A42" s="94"/>
+      <c r="B42" s="97"/>
       <c r="C42" s="12" t="s">
         <v>77</v>
       </c>
@@ -3041,8 +3041,8 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="101"/>
-      <c r="B43" s="103"/>
+      <c r="A43" s="94"/>
+      <c r="B43" s="97"/>
       <c r="C43" s="3" t="s">
         <v>86</v>
       </c>
@@ -3060,8 +3060,8 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="101"/>
-      <c r="B44" s="103"/>
+      <c r="A44" s="94"/>
+      <c r="B44" s="97"/>
       <c r="C44" s="12" t="s">
         <v>88</v>
       </c>
@@ -3079,8 +3079,8 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="101"/>
-      <c r="B45" s="103"/>
+      <c r="A45" s="94"/>
+      <c r="B45" s="97"/>
       <c r="C45" s="3" t="s">
         <v>90</v>
       </c>
@@ -3098,8 +3098,8 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="101"/>
-      <c r="B46" s="103"/>
+      <c r="A46" s="94"/>
+      <c r="B46" s="97"/>
       <c r="C46" s="12" t="s">
         <v>92</v>
       </c>
@@ -3117,8 +3117,8 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="93"/>
-      <c r="B47" s="104"/>
+      <c r="A47" s="95"/>
+      <c r="B47" s="98"/>
       <c r="C47" s="5" t="s">
         <v>94</v>
       </c>
@@ -3137,6 +3137,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="A38:A47"/>
     <mergeCell ref="B38:B47"/>
     <mergeCell ref="A13:A14"/>
@@ -3149,11 +3154,6 @@
     <mergeCell ref="B23:B28"/>
     <mergeCell ref="B29:B37"/>
     <mergeCell ref="A29:A37"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3164,7 +3164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8E41A5-F136-4AC2-820E-22508AAAA400}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -3179,14 +3179,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="120" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
@@ -3209,10 +3209,10 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="118">
+      <c r="B3" s="121">
         <v>21</v>
       </c>
       <c r="C3" s="34" t="s">
@@ -3221,7 +3221,7 @@
       <c r="D3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="132" t="s">
+      <c r="E3" s="135" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="36" t="s">
@@ -3229,29 +3229,29 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="122"/>
-      <c r="B4" s="119"/>
+      <c r="A4" s="125"/>
+      <c r="B4" s="122"/>
       <c r="C4" s="30" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="133"/>
+      <c r="E4" s="110"/>
       <c r="F4" s="36" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="122"/>
-      <c r="B5" s="119"/>
+      <c r="A5" s="125"/>
+      <c r="B5" s="122"/>
       <c r="C5" s="30" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="134" t="s">
+      <c r="E5" s="109" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="36" t="s">
@@ -3259,29 +3259,29 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="122"/>
-      <c r="B6" s="119"/>
+      <c r="A6" s="125"/>
+      <c r="B6" s="122"/>
       <c r="C6" s="30" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="133"/>
+      <c r="E6" s="110"/>
       <c r="F6" s="36" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="122"/>
-      <c r="B7" s="119"/>
+      <c r="A7" s="125"/>
+      <c r="B7" s="122"/>
       <c r="C7" s="30" t="s">
         <v>71</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="134" t="s">
+      <c r="E7" s="109" t="s">
         <v>70</v>
       </c>
       <c r="F7" s="36" t="s">
@@ -3293,15 +3293,15 @@
       <c r="K7" s="24"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="122"/>
-      <c r="B8" s="119"/>
+      <c r="A8" s="125"/>
+      <c r="B8" s="122"/>
       <c r="C8" s="30" t="s">
         <v>80</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="133"/>
+      <c r="E8" s="110"/>
       <c r="F8" s="36" t="s">
         <v>10</v>
       </c>
@@ -3311,15 +3311,15 @@
       <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="122"/>
-      <c r="B9" s="119"/>
+      <c r="A9" s="125"/>
+      <c r="B9" s="122"/>
       <c r="C9" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="146" t="s">
+      <c r="D9" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="134" t="s">
+      <c r="E9" s="109" t="s">
         <v>27</v>
       </c>
       <c r="F9" s="36" t="s">
@@ -3331,15 +3331,15 @@
       <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="122"/>
-      <c r="B10" s="119"/>
+      <c r="A10" s="125"/>
+      <c r="B10" s="122"/>
       <c r="C10" s="30" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="135"/>
+      <c r="E10" s="136"/>
       <c r="F10" s="36" t="s">
         <v>16</v>
       </c>
@@ -3349,15 +3349,15 @@
       <c r="K10" s="24"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="122"/>
-      <c r="B11" s="119"/>
+      <c r="A11" s="125"/>
+      <c r="B11" s="122"/>
       <c r="C11" s="30" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="135"/>
+      <c r="E11" s="136"/>
       <c r="F11" s="36" t="s">
         <v>10</v>
       </c>
@@ -3367,15 +3367,15 @@
       <c r="K11" s="24"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="122"/>
-      <c r="B12" s="119"/>
+      <c r="A12" s="125"/>
+      <c r="B12" s="122"/>
       <c r="C12" s="30" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="135"/>
+      <c r="E12" s="136"/>
       <c r="F12" s="37" t="s">
         <v>16</v>
       </c>
@@ -3385,15 +3385,15 @@
       <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="122"/>
-      <c r="B13" s="119"/>
+      <c r="A13" s="125"/>
+      <c r="B13" s="122"/>
       <c r="C13" s="30" t="s">
         <v>101</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="135"/>
+      <c r="E13" s="136"/>
       <c r="F13" s="36" t="s">
         <v>10</v>
       </c>
@@ -3403,15 +3403,15 @@
       <c r="K13" s="24"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="122"/>
-      <c r="B14" s="119"/>
+      <c r="A14" s="125"/>
+      <c r="B14" s="122"/>
       <c r="C14" s="30" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="135"/>
+      <c r="E14" s="136"/>
       <c r="F14" s="36" t="s">
         <v>10</v>
       </c>
@@ -3421,15 +3421,15 @@
       <c r="K14" s="24"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="122"/>
-      <c r="B15" s="119"/>
+      <c r="A15" s="125"/>
+      <c r="B15" s="122"/>
       <c r="C15" s="30" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="133"/>
+      <c r="E15" s="110"/>
       <c r="F15" s="37" t="s">
         <v>16</v>
       </c>
@@ -3439,15 +3439,15 @@
       <c r="K15" s="24"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="122"/>
-      <c r="B16" s="119"/>
+      <c r="A16" s="125"/>
+      <c r="B16" s="122"/>
       <c r="C16" s="30" t="s">
         <v>51</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="134" t="s">
+      <c r="E16" s="109" t="s">
         <v>69</v>
       </c>
       <c r="F16" s="37" t="s">
@@ -3459,15 +3459,15 @@
       <c r="K16" s="24"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="122"/>
-      <c r="B17" s="119"/>
+      <c r="A17" s="125"/>
+      <c r="B17" s="122"/>
       <c r="C17" s="30" t="s">
         <v>55</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="135"/>
+      <c r="E17" s="136"/>
       <c r="F17" s="37" t="s">
         <v>16</v>
       </c>
@@ -3477,15 +3477,15 @@
       <c r="K17" s="24"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="122"/>
-      <c r="B18" s="119"/>
+      <c r="A18" s="125"/>
+      <c r="B18" s="122"/>
       <c r="C18" s="30" t="s">
         <v>65</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="133"/>
+      <c r="E18" s="110"/>
       <c r="F18" s="37" t="s">
         <v>16</v>
       </c>
@@ -3495,15 +3495,15 @@
       <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="122"/>
-      <c r="B19" s="119"/>
+      <c r="A19" s="125"/>
+      <c r="B19" s="122"/>
       <c r="C19" s="30" t="s">
         <v>75</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="134" t="s">
+      <c r="E19" s="109" t="s">
         <v>74</v>
       </c>
       <c r="F19" s="36" t="s">
@@ -3515,15 +3515,15 @@
       <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="122"/>
-      <c r="B20" s="119"/>
+      <c r="A20" s="125"/>
+      <c r="B20" s="122"/>
       <c r="C20" s="30" t="s">
         <v>79</v>
       </c>
       <c r="D20" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="135"/>
+      <c r="E20" s="136"/>
       <c r="F20" s="36" t="s">
         <v>10</v>
       </c>
@@ -3533,15 +3533,15 @@
       <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="122"/>
-      <c r="B21" s="119"/>
+      <c r="A21" s="125"/>
+      <c r="B21" s="122"/>
       <c r="C21" s="30" t="s">
         <v>86</v>
       </c>
       <c r="D21" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="135"/>
+      <c r="E21" s="136"/>
       <c r="F21" s="48" t="s">
         <v>10</v>
       </c>
@@ -3551,15 +3551,15 @@
       <c r="K21" s="24"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="122"/>
-      <c r="B22" s="119"/>
+      <c r="A22" s="125"/>
+      <c r="B22" s="122"/>
       <c r="C22" s="30" t="s">
         <v>88</v>
       </c>
       <c r="D22" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="135"/>
+      <c r="E22" s="136"/>
       <c r="F22" s="36" t="s">
         <v>10</v>
       </c>
@@ -3569,15 +3569,15 @@
       <c r="K22" s="24"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="123"/>
-      <c r="B23" s="120"/>
+      <c r="A23" s="126"/>
+      <c r="B23" s="123"/>
       <c r="C23" s="38" t="s">
         <v>90</v>
       </c>
       <c r="D23" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="136"/>
+      <c r="E23" s="137"/>
       <c r="F23" s="40" t="s">
         <v>10</v>
       </c>
@@ -3587,10 +3587,10 @@
       <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="127" t="s">
+      <c r="A24" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="124">
+      <c r="B24" s="127">
         <v>21</v>
       </c>
       <c r="C24" s="41" t="s">
@@ -3611,15 +3611,15 @@
       <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="128"/>
-      <c r="B25" s="125"/>
+      <c r="A25" s="131"/>
+      <c r="B25" s="128"/>
       <c r="C25" s="32" t="s">
         <v>43</v>
       </c>
       <c r="D25" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="E25" s="130" t="s">
+      <c r="E25" s="133" t="s">
         <v>42</v>
       </c>
       <c r="F25" s="43" t="s">
@@ -3631,15 +3631,15 @@
       <c r="K25" s="24"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="128"/>
-      <c r="B26" s="125"/>
+      <c r="A26" s="131"/>
+      <c r="B26" s="128"/>
       <c r="C26" s="32" t="s">
         <v>104</v>
       </c>
       <c r="D26" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="E26" s="137"/>
+      <c r="E26" s="138"/>
       <c r="F26" s="43" t="s">
         <v>16</v>
       </c>
@@ -3649,8 +3649,8 @@
       <c r="K26" s="24"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="128"/>
-      <c r="B27" s="125"/>
+      <c r="A27" s="131"/>
+      <c r="B27" s="128"/>
       <c r="C27" s="32" t="s">
         <v>34</v>
       </c>
@@ -3665,15 +3665,15 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="128"/>
-      <c r="B28" s="125"/>
+      <c r="A28" s="131"/>
+      <c r="B28" s="128"/>
       <c r="C28" s="32" t="s">
         <v>44</v>
       </c>
       <c r="D28" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="130" t="s">
+      <c r="E28" s="133" t="s">
         <v>108</v>
       </c>
       <c r="F28" s="43" t="s">
@@ -3681,85 +3681,85 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="128"/>
-      <c r="B29" s="125"/>
+      <c r="A29" s="131"/>
+      <c r="B29" s="128"/>
       <c r="C29" s="32" t="s">
         <v>97</v>
       </c>
       <c r="D29" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="131"/>
+      <c r="E29" s="134"/>
       <c r="F29" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="128"/>
-      <c r="B30" s="125"/>
+      <c r="A30" s="131"/>
+      <c r="B30" s="128"/>
       <c r="C30" s="32" t="s">
         <v>98</v>
       </c>
       <c r="D30" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="131"/>
+      <c r="E30" s="134"/>
       <c r="F30" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="128"/>
-      <c r="B31" s="125"/>
+      <c r="A31" s="131"/>
+      <c r="B31" s="128"/>
       <c r="C31" s="32" t="s">
         <v>102</v>
       </c>
       <c r="D31" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="E31" s="131"/>
+      <c r="E31" s="134"/>
       <c r="F31" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="128"/>
-      <c r="B32" s="125"/>
+      <c r="A32" s="131"/>
+      <c r="B32" s="128"/>
       <c r="C32" s="32" t="s">
         <v>99</v>
       </c>
       <c r="D32" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="131"/>
+      <c r="E32" s="134"/>
       <c r="F32" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="128"/>
-      <c r="B33" s="125"/>
+      <c r="A33" s="131"/>
+      <c r="B33" s="128"/>
       <c r="C33" s="32" t="s">
         <v>46</v>
       </c>
       <c r="D33" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="137"/>
+      <c r="E33" s="138"/>
       <c r="F33" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="128"/>
-      <c r="B34" s="125"/>
+      <c r="A34" s="131"/>
+      <c r="B34" s="128"/>
       <c r="C34" s="32" t="s">
         <v>53</v>
       </c>
       <c r="D34" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="130" t="s">
+      <c r="E34" s="133" t="s">
         <v>69</v>
       </c>
       <c r="F34" s="43" t="s">
@@ -3767,85 +3767,85 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="128"/>
-      <c r="B35" s="125"/>
+      <c r="A35" s="131"/>
+      <c r="B35" s="128"/>
       <c r="C35" s="32" t="s">
         <v>57</v>
       </c>
       <c r="D35" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="131"/>
+      <c r="E35" s="134"/>
       <c r="F35" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="128"/>
-      <c r="B36" s="125"/>
+      <c r="A36" s="131"/>
+      <c r="B36" s="128"/>
       <c r="C36" s="32" t="s">
         <v>59</v>
       </c>
       <c r="D36" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="131"/>
+      <c r="E36" s="134"/>
       <c r="F36" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="128"/>
-      <c r="B37" s="125"/>
+      <c r="A37" s="131"/>
+      <c r="B37" s="128"/>
       <c r="C37" s="32" t="s">
         <v>61</v>
       </c>
       <c r="D37" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="131"/>
+      <c r="E37" s="134"/>
       <c r="F37" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="128"/>
-      <c r="B38" s="125"/>
+      <c r="A38" s="131"/>
+      <c r="B38" s="128"/>
       <c r="C38" s="32" t="s">
         <v>63</v>
       </c>
       <c r="D38" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="E38" s="131"/>
+      <c r="E38" s="134"/>
       <c r="F38" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="128"/>
-      <c r="B39" s="125"/>
+      <c r="A39" s="131"/>
+      <c r="B39" s="128"/>
       <c r="C39" s="32" t="s">
         <v>67</v>
       </c>
       <c r="D39" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="E39" s="137"/>
+      <c r="E39" s="138"/>
       <c r="F39" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="128"/>
-      <c r="B40" s="125"/>
+      <c r="A40" s="131"/>
+      <c r="B40" s="128"/>
       <c r="C40" s="32" t="s">
         <v>81</v>
       </c>
       <c r="D40" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="E40" s="130" t="s">
+      <c r="E40" s="133" t="s">
         <v>74</v>
       </c>
       <c r="F40" s="43" t="s">
@@ -3855,67 +3855,67 @@
       <c r="H40" s="24"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="128"/>
-      <c r="B41" s="125"/>
+      <c r="A41" s="131"/>
+      <c r="B41" s="128"/>
       <c r="C41" s="32" t="s">
         <v>83</v>
       </c>
       <c r="D41" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="E41" s="131"/>
+      <c r="E41" s="134"/>
       <c r="F41" s="43" t="s">
         <v>10</v>
       </c>
       <c r="G41" s="45"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="128"/>
-      <c r="B42" s="125"/>
+      <c r="A42" s="131"/>
+      <c r="B42" s="128"/>
       <c r="C42" s="32" t="s">
         <v>77</v>
       </c>
       <c r="D42" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="E42" s="131"/>
+      <c r="E42" s="134"/>
       <c r="F42" s="44" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="128"/>
-      <c r="B43" s="125"/>
+      <c r="A43" s="131"/>
+      <c r="B43" s="128"/>
       <c r="C43" s="32" t="s">
         <v>92</v>
       </c>
       <c r="D43" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="E43" s="131"/>
+      <c r="E43" s="134"/>
       <c r="F43" s="43" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="129"/>
-      <c r="B44" s="126"/>
+      <c r="A44" s="132"/>
+      <c r="B44" s="129"/>
       <c r="C44" s="66" t="s">
         <v>94</v>
       </c>
       <c r="D44" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="E44" s="131"/>
+      <c r="E44" s="134"/>
       <c r="F44" s="68" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="108" t="s">
+      <c r="A45" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="111">
+      <c r="B45" s="114">
         <v>2</v>
       </c>
       <c r="C45" s="69" t="s">
@@ -3924,7 +3924,7 @@
       <c r="D45" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="E45" s="114" t="s">
+      <c r="E45" s="117" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="71" t="s">
@@ -3932,40 +3932,35 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="109"/>
-      <c r="B46" s="112"/>
+      <c r="A46" s="112"/>
+      <c r="B46" s="115"/>
       <c r="C46" s="64" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="E46" s="115"/>
+      <c r="E46" s="118"/>
       <c r="F46" s="72" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="110"/>
-      <c r="B47" s="113"/>
+      <c r="A47" s="113"/>
+      <c r="B47" s="116"/>
       <c r="C47" s="73" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="E47" s="116"/>
+      <c r="E47" s="119"/>
       <c r="F47" s="75" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="E45:E47"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B3:B23"/>
     <mergeCell ref="A3:A23"/>
@@ -3979,6 +3974,11 @@
     <mergeCell ref="E28:E33"/>
     <mergeCell ref="E34:E39"/>
     <mergeCell ref="E9:E15"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="E45:E47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4003,13 +4003,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="139" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
@@ -4029,7 +4029,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="139" t="s">
+      <c r="A3" s="140" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="54" t="s">
@@ -4038,7 +4038,7 @@
       <c r="C3" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="144" t="s">
+      <c r="D3" s="145" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="62" t="s">
@@ -4046,59 +4046,59 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="140"/>
+      <c r="A4" s="141"/>
       <c r="B4" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="144"/>
+      <c r="D4" s="145"/>
       <c r="E4" s="61" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="140"/>
+      <c r="A5" s="141"/>
       <c r="B5" s="55" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="144"/>
+      <c r="D5" s="145"/>
       <c r="E5" s="60" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="140"/>
+      <c r="A6" s="141"/>
       <c r="B6" s="27" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="144"/>
+      <c r="D6" s="145"/>
       <c r="E6" s="60" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="140"/>
+      <c r="A7" s="141"/>
       <c r="B7" s="55" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="145"/>
+      <c r="D7" s="146"/>
       <c r="E7" s="52" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="141"/>
+      <c r="A8" s="142"/>
       <c r="B8" s="27" t="s">
         <v>34</v>
       </c>
@@ -4113,7 +4113,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="142" t="s">
+      <c r="A9" s="143" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="27" t="s">
@@ -4130,7 +4130,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="143"/>
+      <c r="A10" s="144"/>
       <c r="B10" s="56" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Se identifican dos nuevos CU para el módulo de citas: EM-Citas-CU1.4 Consultar Citas Canceladas y EM-Citas-CU1.4.1 Eliminar Citas Canceladas. Se modifica maquetas de citas para agregar mockups de los nuevos CU y se adaptan los anteriores para adaptarlos con los nuevos. Se exportan imágenes de las maquetas de citas y se modifica PlaneaciónCU para dar paso a los mismos
</commit_message>
<xml_diff>
--- a/Documentacion Tecnica/PlaneacionCU/Planeacion.xlsx
+++ b/Documentacion Tecnica/PlaneacionCU/Planeacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8.1\Desktop\ESCOMobile TT2\ESCOMobile\Documentacion Tecnica\PlaneacionCU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD66125-AFF0-42FC-B115-9C516B1BAADE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB57B37C-B895-4D4C-9333-E670A7DDBD2F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{6BEE2BBB-66B6-49FE-B5FF-8E26273E1384}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="129">
   <si>
     <t>Módulo</t>
   </si>
@@ -407,6 +407,18 @@
   </si>
   <si>
     <t xml:space="preserve">Alumno, profesor. </t>
+  </si>
+  <si>
+    <t>EM-Citas-CU1.4</t>
+  </si>
+  <si>
+    <t>Consultar Citas Canceladas</t>
+  </si>
+  <si>
+    <t>Eliminar Citas Canceladas</t>
+  </si>
+  <si>
+    <t>EM-Citas-CU1.4.1</t>
   </si>
 </sst>
 </file>
@@ -536,7 +548,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="78">
+  <borders count="84">
     <border>
       <left/>
       <right/>
@@ -893,17 +905,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="9" tint="-0.249977111117893"/>
       </left>
@@ -952,17 +953,6 @@
       </top>
       <bottom style="thin">
         <color theme="9" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1509,11 +1499,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="8" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="8" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="8" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="8" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="8" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="8" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="8" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="8" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="8" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="9" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="9" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="9" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1572,128 +1670,128 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="59" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="64" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="65" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="62" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="63" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="71" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="72" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="69" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="70" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="71" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="72" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="73" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="73" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="72" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="76" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="76" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="77" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="77" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1710,12 +1808,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1725,15 +1844,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1743,131 +1853,155 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="76" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="77" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="78" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="79" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="80" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="81" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="82" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="83" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2183,10 +2317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9913E36-BDE9-470A-AFF3-2C8FCCD03D79}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2202,15 +2336,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2236,10 +2370,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="99">
+      <c r="B3" s="95">
         <v>6</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -2259,8 +2393,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="106"/>
-      <c r="B4" s="101"/>
+      <c r="A4" s="98"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
@@ -2278,8 +2412,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="106"/>
-      <c r="B5" s="101"/>
+      <c r="A5" s="98"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
@@ -2297,8 +2431,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="106"/>
-      <c r="B6" s="101"/>
+      <c r="A6" s="98"/>
+      <c r="B6" s="100"/>
       <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
@@ -2316,8 +2450,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="106"/>
-      <c r="B7" s="101"/>
+      <c r="A7" s="98"/>
+      <c r="B7" s="100"/>
       <c r="C7" s="27" t="s">
         <v>11</v>
       </c>
@@ -2335,8 +2469,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="107"/>
-      <c r="B8" s="100"/>
+      <c r="A8" s="99"/>
+      <c r="B8" s="96"/>
       <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
@@ -2358,7 +2492,7 @@
       <c r="A9" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="99">
+      <c r="B9" s="95">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2378,8 +2512,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="95"/>
-      <c r="B10" s="100"/>
+      <c r="A10" s="94"/>
+      <c r="B10" s="96"/>
       <c r="C10" s="18" t="s">
         <v>24</v>
       </c>
@@ -2400,7 +2534,7 @@
       <c r="A11" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="99">
+      <c r="B11" s="95">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2420,8 +2554,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="95"/>
-      <c r="B12" s="100"/>
+      <c r="A12" s="94"/>
+      <c r="B12" s="96"/>
       <c r="C12" s="18" t="s">
         <v>104</v>
       </c>
@@ -2442,7 +2576,7 @@
       <c r="A13" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="99">
+      <c r="B13" s="95">
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2462,8 +2596,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="95"/>
-      <c r="B14" s="100"/>
+      <c r="A14" s="94"/>
+      <c r="B14" s="96"/>
       <c r="C14" s="18" t="s">
         <v>80</v>
       </c>
@@ -2481,11 +2615,11 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="93" t="s">
+      <c r="A15" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="99">
-        <v>8</v>
+      <c r="B15" s="95">
+        <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>28</v>
@@ -2504,8 +2638,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="94"/>
-      <c r="B16" s="101"/>
+      <c r="A16" s="98"/>
+      <c r="B16" s="100"/>
       <c r="C16" s="12" t="s">
         <v>30</v>
       </c>
@@ -2523,8 +2657,8 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="94"/>
-      <c r="B17" s="101"/>
+      <c r="A17" s="98"/>
+      <c r="B17" s="100"/>
       <c r="C17" s="3" t="s">
         <v>32</v>
       </c>
@@ -2542,8 +2676,8 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="94"/>
-      <c r="B18" s="101"/>
+      <c r="A18" s="98"/>
+      <c r="B18" s="100"/>
       <c r="C18" s="12" t="s">
         <v>34</v>
       </c>
@@ -2561,8 +2695,8 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="94"/>
-      <c r="B19" s="101"/>
+      <c r="A19" s="98"/>
+      <c r="B19" s="100"/>
       <c r="C19" s="26" t="s">
         <v>36</v>
       </c>
@@ -2580,8 +2714,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="94"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="98"/>
+      <c r="B20" s="100"/>
       <c r="C20" s="3" t="s">
         <v>101</v>
       </c>
@@ -2598,9 +2732,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="94"/>
-      <c r="B21" s="101"/>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="99"/>
+      <c r="B21" s="96"/>
       <c r="C21" s="12" t="s">
         <v>38</v>
       </c>
@@ -2617,81 +2751,85 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="95"/>
-      <c r="B22" s="100"/>
-      <c r="C22" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="84" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="90" t="s">
-        <v>118</v>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="106" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="103">
+        <v>6</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="85" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="88" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="102" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="96">
-        <v>6</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="17" t="s">
+      <c r="A23" s="107"/>
+      <c r="B23" s="104"/>
+      <c r="C23" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="85" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="88" t="s">
+      <c r="F23" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="89" t="s">
         <v>120</v>
       </c>
+      <c r="H23" s="24"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="103"/>
-      <c r="B24" s="97"/>
-      <c r="C24" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="4" t="s">
+      <c r="A24" s="107"/>
+      <c r="B24" s="104"/>
+      <c r="C24" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="79" t="s">
+      <c r="F24" s="78" t="s">
         <v>16</v>
       </c>
       <c r="G24" s="89" t="s">
         <v>120</v>
       </c>
       <c r="H24" s="24"/>
-      <c r="I24" s="25"/>
+      <c r="I24" s="24"/>
       <c r="J24" s="24"/>
       <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="103"/>
-      <c r="B25" s="97"/>
-      <c r="C25" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="10" t="s">
+      <c r="A25" s="107"/>
+      <c r="B25" s="104"/>
+      <c r="C25" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F25" s="78" t="s">
@@ -2706,15 +2844,15 @@
       <c r="K25" s="24"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="103"/>
-      <c r="B26" s="97"/>
-      <c r="C26" s="27" t="s">
-        <v>102</v>
+      <c r="A26" s="107"/>
+      <c r="B26" s="104"/>
+      <c r="C26" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="E26" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F26" s="78" t="s">
@@ -2723,85 +2861,81 @@
       <c r="G26" s="89" t="s">
         <v>120</v>
       </c>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="103"/>
-      <c r="B27" s="97"/>
-      <c r="C27" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="4" t="s">
+    </row>
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="108"/>
+      <c r="B27" s="105"/>
+      <c r="C27" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="78" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="89" t="s">
+      <c r="F27" s="83" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="90" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="104"/>
-      <c r="B28" s="98"/>
-      <c r="C28" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="20" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="145" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="95">
+        <v>11</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="88" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="146"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F28" s="83" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="90" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="102" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="99">
+      <c r="F29" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="89" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="146"/>
+      <c r="B30" s="100"/>
+      <c r="C30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="82" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="88" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="103"/>
-      <c r="B30" s="101"/>
-      <c r="C30" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="78" t="s">
+      <c r="F30" s="79" t="s">
         <v>16</v>
       </c>
       <c r="G30" s="89" t="s">
@@ -2809,56 +2943,56 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="103"/>
-      <c r="B31" s="101"/>
-      <c r="C31" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="79" t="s">
+      <c r="A31" s="146"/>
+      <c r="B31" s="100"/>
+      <c r="C31" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="78" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="89" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="146"/>
+      <c r="B32" s="100"/>
+      <c r="C32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="89" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="103"/>
-      <c r="B32" s="101"/>
-      <c r="C32" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E32" s="10" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="146"/>
+      <c r="B33" s="100"/>
+      <c r="C33" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F32" s="78" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="89" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="103"/>
-      <c r="B33" s="101"/>
-      <c r="C33" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="79" t="s">
+      <c r="F33" s="78" t="s">
         <v>16</v>
       </c>
       <c r="G33" s="89" t="s">
@@ -2866,18 +3000,18 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="103"/>
-      <c r="B34" s="101"/>
-      <c r="C34" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E34" s="10" t="s">
+      <c r="A34" s="146"/>
+      <c r="B34" s="100"/>
+      <c r="C34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F34" s="78" t="s">
+      <c r="F34" s="79" t="s">
         <v>16</v>
       </c>
       <c r="G34" s="89" t="s">
@@ -2885,117 +3019,117 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="103"/>
-      <c r="B35" s="101"/>
-      <c r="C35" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="A35" s="146"/>
+      <c r="B35" s="100"/>
+      <c r="C35" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="149" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="89" t="s">
+      <c r="F35" s="151" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="144" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="103"/>
-      <c r="B36" s="101"/>
-      <c r="C36" s="12" t="s">
+      <c r="A36" s="146"/>
+      <c r="B36" s="148"/>
+      <c r="C36" s="153" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="154" t="s">
+        <v>127</v>
+      </c>
+      <c r="E36" s="155" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="156" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="157" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="146"/>
+      <c r="B37" s="148"/>
+      <c r="C37" s="153" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D37" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E37" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="78" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="89" t="s">
+      <c r="F37" s="156" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="157" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="104"/>
-      <c r="B37" s="100"/>
-      <c r="C37" s="5" t="s">
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="147"/>
+      <c r="B38" s="96"/>
+      <c r="C38" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D38" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E38" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F37" s="84" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="90" t="s">
+      <c r="F38" s="84" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" s="152" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="93" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="93" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="96">
-        <v>10</v>
-      </c>
-      <c r="C38" s="15" t="s">
+      <c r="B39" s="103">
+        <v>10</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D39" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E39" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="76" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" s="88" t="s">
+      <c r="F39" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="88" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="94"/>
-      <c r="B39" s="97"/>
-      <c r="C39" s="3" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="102"/>
+      <c r="B40" s="104"/>
+      <c r="C40" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D40" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E40" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F39" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="89" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="94"/>
-      <c r="B40" s="97"/>
-      <c r="C40" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" s="86" t="s">
+      <c r="F40" s="77" t="s">
         <v>10</v>
       </c>
       <c r="G40" s="89" t="s">
@@ -3003,18 +3137,18 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="94"/>
-      <c r="B41" s="97"/>
-      <c r="C41" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="E41" s="4" t="s">
+      <c r="A41" s="102"/>
+      <c r="B41" s="104"/>
+      <c r="C41" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F41" s="77" t="s">
+      <c r="F41" s="86" t="s">
         <v>10</v>
       </c>
       <c r="G41" s="89" t="s">
@@ -3022,18 +3156,18 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="94"/>
-      <c r="B42" s="97"/>
-      <c r="C42" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="E42" s="10" t="s">
+      <c r="A42" s="102"/>
+      <c r="B42" s="104"/>
+      <c r="C42" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F42" s="86" t="s">
+      <c r="F42" s="77" t="s">
         <v>10</v>
       </c>
       <c r="G42" s="89" t="s">
@@ -3041,18 +3175,18 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="94"/>
-      <c r="B43" s="97"/>
-      <c r="C43" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="77" t="s">
+      <c r="A43" s="102"/>
+      <c r="B43" s="104"/>
+      <c r="C43" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="86" t="s">
         <v>10</v>
       </c>
       <c r="G43" s="89" t="s">
@@ -3060,18 +3194,18 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="94"/>
-      <c r="B44" s="97"/>
-      <c r="C44" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="E44" s="10" t="s">
+      <c r="A44" s="102"/>
+      <c r="B44" s="104"/>
+      <c r="C44" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F44" s="86" t="s">
+      <c r="F44" s="77" t="s">
         <v>10</v>
       </c>
       <c r="G44" s="89" t="s">
@@ -3079,18 +3213,18 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="94"/>
-      <c r="B45" s="97"/>
-      <c r="C45" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="E45" s="4" t="s">
+      <c r="A45" s="102"/>
+      <c r="B45" s="104"/>
+      <c r="C45" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F45" s="77" t="s">
+      <c r="F45" s="86" t="s">
         <v>10</v>
       </c>
       <c r="G45" s="89" t="s">
@@ -3098,62 +3232,81 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="94"/>
-      <c r="B46" s="97"/>
-      <c r="C46" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" s="86" t="s">
+      <c r="A46" s="102"/>
+      <c r="B46" s="104"/>
+      <c r="C46" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="77" t="s">
         <v>10</v>
       </c>
       <c r="G46" s="89" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="95"/>
-      <c r="B47" s="98"/>
-      <c r="C47" s="5" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="102"/>
+      <c r="B47" s="104"/>
+      <c r="C47" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="89" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="94"/>
+      <c r="B48" s="105"/>
+      <c r="C48" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D48" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="E48" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F47" s="87" t="s">
-        <v>10</v>
-      </c>
-      <c r="G47" s="90" t="s">
+      <c r="F48" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="90" t="s">
         <v>121</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A39:A48"/>
+    <mergeCell ref="B39:B48"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="A28:A38"/>
+    <mergeCell ref="B28:B38"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="B15:B21"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A38:A47"/>
-    <mergeCell ref="B38:B47"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A15:A22"/>
-    <mergeCell ref="B15:B22"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="B29:B37"/>
-    <mergeCell ref="A29:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3162,10 +3315,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8E41A5-F136-4AC2-820E-22508AAAA400}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3179,14 +3332,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="109" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
@@ -3209,11 +3362,11 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="124" t="s">
+      <c r="A3" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="121">
-        <v>21</v>
+      <c r="B3" s="110">
+        <v>20</v>
       </c>
       <c r="C3" s="34" t="s">
         <v>7</v>
@@ -3221,7 +3374,7 @@
       <c r="D3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="135" t="s">
+      <c r="E3" s="121" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="36" t="s">
@@ -3229,29 +3382,29 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="125"/>
-      <c r="B4" s="122"/>
+      <c r="A4" s="159"/>
+      <c r="B4" s="111"/>
       <c r="C4" s="30" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="110"/>
+      <c r="E4" s="122"/>
       <c r="F4" s="36" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="125"/>
-      <c r="B5" s="122"/>
+      <c r="A5" s="159"/>
+      <c r="B5" s="111"/>
       <c r="C5" s="30" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="109" t="s">
+      <c r="E5" s="123" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="36" t="s">
@@ -3259,29 +3412,29 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="125"/>
-      <c r="B6" s="122"/>
+      <c r="A6" s="159"/>
+      <c r="B6" s="111"/>
       <c r="C6" s="30" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="110"/>
+      <c r="E6" s="122"/>
       <c r="F6" s="36" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="125"/>
-      <c r="B7" s="122"/>
+      <c r="A7" s="159"/>
+      <c r="B7" s="111"/>
       <c r="C7" s="30" t="s">
         <v>71</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="109" t="s">
+      <c r="E7" s="123" t="s">
         <v>70</v>
       </c>
       <c r="F7" s="36" t="s">
@@ -3293,15 +3446,15 @@
       <c r="K7" s="24"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="125"/>
-      <c r="B8" s="122"/>
+      <c r="A8" s="159"/>
+      <c r="B8" s="111"/>
       <c r="C8" s="30" t="s">
         <v>80</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="110"/>
+      <c r="E8" s="122"/>
       <c r="F8" s="36" t="s">
         <v>10</v>
       </c>
@@ -3311,15 +3464,15 @@
       <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="125"/>
-      <c r="B9" s="122"/>
+      <c r="A9" s="159"/>
+      <c r="B9" s="111"/>
       <c r="C9" s="30" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="109" t="s">
+      <c r="E9" s="123" t="s">
         <v>27</v>
       </c>
       <c r="F9" s="36" t="s">
@@ -3331,15 +3484,15 @@
       <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="125"/>
-      <c r="B10" s="122"/>
+      <c r="A10" s="159"/>
+      <c r="B10" s="111"/>
       <c r="C10" s="30" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="136"/>
+      <c r="E10" s="124"/>
       <c r="F10" s="36" t="s">
         <v>16</v>
       </c>
@@ -3349,15 +3502,15 @@
       <c r="K10" s="24"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="125"/>
-      <c r="B11" s="122"/>
+      <c r="A11" s="159"/>
+      <c r="B11" s="111"/>
       <c r="C11" s="30" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="136"/>
+      <c r="E11" s="124"/>
       <c r="F11" s="36" t="s">
         <v>10</v>
       </c>
@@ -3367,15 +3520,15 @@
       <c r="K11" s="24"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="125"/>
-      <c r="B12" s="122"/>
+      <c r="A12" s="159"/>
+      <c r="B12" s="111"/>
       <c r="C12" s="30" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="136"/>
+      <c r="E12" s="124"/>
       <c r="F12" s="37" t="s">
         <v>16</v>
       </c>
@@ -3385,15 +3538,15 @@
       <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="125"/>
-      <c r="B13" s="122"/>
+      <c r="A13" s="159"/>
+      <c r="B13" s="111"/>
       <c r="C13" s="30" t="s">
         <v>101</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="136"/>
+      <c r="E13" s="124"/>
       <c r="F13" s="36" t="s">
         <v>10</v>
       </c>
@@ -3403,15 +3556,15 @@
       <c r="K13" s="24"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="125"/>
-      <c r="B14" s="122"/>
+      <c r="A14" s="159"/>
+      <c r="B14" s="111"/>
       <c r="C14" s="30" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="136"/>
+      <c r="E14" s="122"/>
       <c r="F14" s="36" t="s">
         <v>10</v>
       </c>
@@ -3421,15 +3574,17 @@
       <c r="K14" s="24"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="125"/>
-      <c r="B15" s="122"/>
+      <c r="A15" s="159"/>
+      <c r="B15" s="111"/>
       <c r="C15" s="30" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="110"/>
+        <v>52</v>
+      </c>
+      <c r="E15" s="123" t="s">
+        <v>69</v>
+      </c>
       <c r="F15" s="37" t="s">
         <v>16</v>
       </c>
@@ -3439,17 +3594,15 @@
       <c r="K15" s="24"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="125"/>
-      <c r="B16" s="122"/>
+      <c r="A16" s="159"/>
+      <c r="B16" s="111"/>
       <c r="C16" s="30" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="109" t="s">
-        <v>69</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E16" s="124"/>
       <c r="F16" s="37" t="s">
         <v>16</v>
       </c>
@@ -3459,15 +3612,15 @@
       <c r="K16" s="24"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="125"/>
-      <c r="B17" s="122"/>
+      <c r="A17" s="159"/>
+      <c r="B17" s="111"/>
       <c r="C17" s="30" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="136"/>
+        <v>66</v>
+      </c>
+      <c r="E17" s="122"/>
       <c r="F17" s="37" t="s">
         <v>16</v>
       </c>
@@ -3477,17 +3630,19 @@
       <c r="K17" s="24"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="125"/>
-      <c r="B18" s="122"/>
+      <c r="A18" s="159"/>
+      <c r="B18" s="111"/>
       <c r="C18" s="30" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="110"/>
-      <c r="F18" s="37" t="s">
-        <v>16</v>
+        <v>76</v>
+      </c>
+      <c r="E18" s="123" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>10</v>
       </c>
       <c r="H18" s="24"/>
       <c r="I18" s="24"/>
@@ -3495,17 +3650,15 @@
       <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="125"/>
-      <c r="B19" s="122"/>
+      <c r="A19" s="159"/>
+      <c r="B19" s="111"/>
       <c r="C19" s="30" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="109" t="s">
-        <v>74</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="E19" s="124"/>
       <c r="F19" s="36" t="s">
         <v>10</v>
       </c>
@@ -3515,16 +3668,16 @@
       <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="125"/>
-      <c r="B20" s="122"/>
+      <c r="A20" s="159"/>
+      <c r="B20" s="111"/>
       <c r="C20" s="30" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" s="136"/>
-      <c r="F20" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="124"/>
+      <c r="F20" s="48" t="s">
         <v>10</v>
       </c>
       <c r="H20" s="24"/>
@@ -3533,16 +3686,16 @@
       <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="125"/>
-      <c r="B21" s="122"/>
+      <c r="A21" s="159"/>
+      <c r="B21" s="111"/>
       <c r="C21" s="30" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="136"/>
-      <c r="F21" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="124"/>
+      <c r="F21" s="36" t="s">
         <v>10</v>
       </c>
       <c r="H21" s="24"/>
@@ -3550,17 +3703,17 @@
       <c r="J21" s="24"/>
       <c r="K21" s="24"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="125"/>
-      <c r="B22" s="122"/>
-      <c r="C22" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" s="136"/>
-      <c r="F22" s="36" t="s">
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="160"/>
+      <c r="B22" s="112"/>
+      <c r="C22" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="125"/>
+      <c r="F22" s="40" t="s">
         <v>10</v>
       </c>
       <c r="H22" s="24"/>
@@ -3568,17 +3721,23 @@
       <c r="J22" s="24"/>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="126"/>
-      <c r="B23" s="123"/>
-      <c r="C23" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="137"/>
-      <c r="F23" s="40" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="116" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="113">
+        <v>23</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="63" t="s">
         <v>10</v>
       </c>
       <c r="H23" s="24"/>
@@ -3587,23 +3746,19 @@
       <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="130" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="127">
-        <v>21</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="63" t="s">
-        <v>10</v>
+      <c r="A24" s="117"/>
+      <c r="B24" s="114"/>
+      <c r="C24" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="119" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="43" t="s">
+        <v>16</v>
       </c>
       <c r="H24" s="24"/>
       <c r="I24" s="24"/>
@@ -3611,17 +3766,15 @@
       <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="131"/>
-      <c r="B25" s="128"/>
+      <c r="A25" s="117"/>
+      <c r="B25" s="114"/>
       <c r="C25" s="32" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="E25" s="133" t="s">
-        <v>42</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="E25" s="126"/>
       <c r="F25" s="43" t="s">
         <v>16</v>
       </c>
@@ -3631,354 +3784,364 @@
       <c r="K25" s="24"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="131"/>
-      <c r="B26" s="128"/>
+      <c r="A26" s="117"/>
+      <c r="B26" s="114"/>
       <c r="C26" s="32" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="E26" s="138"/>
-      <c r="F26" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
+        <v>35</v>
+      </c>
+      <c r="E26" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="44" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="131"/>
-      <c r="B27" s="128"/>
+      <c r="A27" s="117"/>
+      <c r="B27" s="114"/>
       <c r="C27" s="32" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D27" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="44" t="s">
-        <v>10</v>
+        <v>47</v>
+      </c>
+      <c r="E27" s="119" t="s">
+        <v>108</v>
+      </c>
+      <c r="F27" s="43" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="131"/>
-      <c r="B28" s="128"/>
+      <c r="A28" s="117"/>
+      <c r="B28" s="114"/>
       <c r="C28" s="32" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" s="133" t="s">
-        <v>108</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E28" s="120"/>
       <c r="F28" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="131"/>
-      <c r="B29" s="128"/>
+      <c r="A29" s="117"/>
+      <c r="B29" s="114"/>
       <c r="C29" s="32" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" s="134"/>
+        <v>49</v>
+      </c>
+      <c r="E29" s="120"/>
       <c r="F29" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="131"/>
-      <c r="B30" s="128"/>
+      <c r="A30" s="117"/>
+      <c r="B30" s="114"/>
       <c r="C30" s="32" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" s="134"/>
+        <v>103</v>
+      </c>
+      <c r="E30" s="120"/>
       <c r="F30" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="131"/>
-      <c r="B31" s="128"/>
+      <c r="A31" s="117"/>
+      <c r="B31" s="114"/>
       <c r="C31" s="32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="E31" s="134"/>
+        <v>45</v>
+      </c>
+      <c r="E31" s="120"/>
       <c r="F31" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="131"/>
-      <c r="B32" s="128"/>
+      <c r="A32" s="117"/>
+      <c r="B32" s="114"/>
       <c r="C32" s="32" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="D32" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="E32" s="134"/>
+        <v>50</v>
+      </c>
+      <c r="E32" s="126"/>
       <c r="F32" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="131"/>
-      <c r="B33" s="128"/>
+      <c r="A33" s="117"/>
+      <c r="B33" s="114"/>
       <c r="C33" s="32" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D33" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33" s="138"/>
+        <v>54</v>
+      </c>
+      <c r="E33" s="119" t="s">
+        <v>69</v>
+      </c>
       <c r="F33" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="131"/>
-      <c r="B34" s="128"/>
+      <c r="A34" s="117"/>
+      <c r="B34" s="114"/>
       <c r="C34" s="32" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D34" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="E34" s="133" t="s">
-        <v>69</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E34" s="120"/>
       <c r="F34" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="131"/>
-      <c r="B35" s="128"/>
+      <c r="A35" s="117"/>
+      <c r="B35" s="114"/>
       <c r="C35" s="32" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="134"/>
+        <v>60</v>
+      </c>
+      <c r="E35" s="120"/>
       <c r="F35" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="131"/>
-      <c r="B36" s="128"/>
+      <c r="A36" s="117"/>
+      <c r="B36" s="114"/>
       <c r="C36" s="32" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" s="134"/>
+        <v>62</v>
+      </c>
+      <c r="E36" s="120"/>
       <c r="F36" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="131"/>
-      <c r="B37" s="128"/>
+      <c r="A37" s="117"/>
+      <c r="B37" s="114"/>
       <c r="C37" s="32" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="E37" s="134"/>
+        <v>64</v>
+      </c>
+      <c r="E37" s="120"/>
       <c r="F37" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="131"/>
-      <c r="B38" s="128"/>
+      <c r="A38" s="117"/>
+      <c r="B38" s="114"/>
       <c r="C38" s="32" t="s">
-        <v>63</v>
+        <v>125</v>
       </c>
       <c r="D38" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="E38" s="134"/>
+        <v>126</v>
+      </c>
+      <c r="E38" s="120"/>
       <c r="F38" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="131"/>
-      <c r="B39" s="128"/>
+      <c r="A39" s="117"/>
+      <c r="B39" s="114"/>
       <c r="C39" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="E39" s="120"/>
+      <c r="F39" s="43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="117"/>
+      <c r="B40" s="114"/>
+      <c r="C40" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="D39" s="33" t="s">
+      <c r="D40" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="E39" s="138"/>
-      <c r="F39" s="43" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="131"/>
-      <c r="B40" s="128"/>
-      <c r="C40" s="32" t="s">
+      <c r="E40" s="126"/>
+      <c r="F40" s="43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="117"/>
+      <c r="B41" s="114"/>
+      <c r="C41" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="D40" s="33" t="s">
+      <c r="D41" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="E40" s="133" t="s">
+      <c r="E41" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="F40" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="G40" s="45"/>
-      <c r="H40" s="24"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="131"/>
-      <c r="B41" s="128"/>
-      <c r="C41" s="32" t="s">
+      <c r="F41" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="45"/>
+      <c r="H41" s="24"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="117"/>
+      <c r="B42" s="114"/>
+      <c r="C42" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="D41" s="33" t="s">
+      <c r="D42" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="E41" s="134"/>
-      <c r="F41" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="G41" s="45"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="131"/>
-      <c r="B42" s="128"/>
-      <c r="C42" s="32" t="s">
+      <c r="E42" s="120"/>
+      <c r="F42" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="45"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="117"/>
+      <c r="B43" s="114"/>
+      <c r="C43" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="D42" s="33" t="s">
+      <c r="D43" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="E42" s="134"/>
-      <c r="F42" s="44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="131"/>
-      <c r="B43" s="128"/>
-      <c r="C43" s="32" t="s">
+      <c r="E43" s="120"/>
+      <c r="F43" s="44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="117"/>
+      <c r="B44" s="114"/>
+      <c r="C44" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="D43" s="33" t="s">
+      <c r="D44" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="E43" s="134"/>
-      <c r="F43" s="43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="132"/>
-      <c r="B44" s="129"/>
-      <c r="C44" s="66" t="s">
+      <c r="E44" s="120"/>
+      <c r="F44" s="43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="118"/>
+      <c r="B45" s="115"/>
+      <c r="C45" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="67" t="s">
+      <c r="D45" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="E44" s="134"/>
-      <c r="F44" s="68" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="111" t="s">
+      <c r="E45" s="120"/>
+      <c r="F45" s="68" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="114">
+      <c r="B46" s="130">
         <v>2</v>
       </c>
-      <c r="C45" s="69" t="s">
+      <c r="C46" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="D45" s="70" t="s">
+      <c r="D46" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="E45" s="117" t="s">
+      <c r="E46" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="F45" s="71" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="112"/>
-      <c r="B46" s="115"/>
-      <c r="C46" s="64" t="s">
+      <c r="F46" s="71" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="128"/>
+      <c r="B47" s="131"/>
+      <c r="C47" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="65" t="s">
+      <c r="D47" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="E46" s="118"/>
-      <c r="F46" s="72" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="113"/>
-      <c r="B47" s="116"/>
-      <c r="C47" s="73" t="s">
+      <c r="E47" s="134"/>
+      <c r="F47" s="72" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="129"/>
+      <c r="B48" s="132"/>
+      <c r="C48" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="74" t="s">
+      <c r="D48" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="E47" s="119"/>
-      <c r="F47" s="75" t="s">
+      <c r="E48" s="135"/>
+      <c r="F48" s="75" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="B3:B22"/>
+    <mergeCell ref="A3:A22"/>
+    <mergeCell ref="E33:E40"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B3:B23"/>
-    <mergeCell ref="A3:A23"/>
-    <mergeCell ref="B24:B44"/>
-    <mergeCell ref="A24:A44"/>
-    <mergeCell ref="E40:E44"/>
+    <mergeCell ref="B23:B45"/>
+    <mergeCell ref="A23:A45"/>
+    <mergeCell ref="E41:E45"/>
     <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="E19:E23"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E28:E33"/>
-    <mergeCell ref="E34:E39"/>
-    <mergeCell ref="E9:E15"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="E18:E22"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E27:E32"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="E45:E47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4003,13 +4166,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="136" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
@@ -4029,7 +4192,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="140" t="s">
+      <c r="A3" s="137" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="54" t="s">
@@ -4038,7 +4201,7 @@
       <c r="C3" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="145" t="s">
+      <c r="D3" s="142" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="62" t="s">
@@ -4046,59 +4209,59 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="141"/>
+      <c r="A4" s="138"/>
       <c r="B4" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="145"/>
+      <c r="D4" s="142"/>
       <c r="E4" s="61" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="141"/>
+      <c r="A5" s="138"/>
       <c r="B5" s="55" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="145"/>
+      <c r="D5" s="142"/>
       <c r="E5" s="60" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="141"/>
+      <c r="A6" s="138"/>
       <c r="B6" s="27" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="145"/>
+      <c r="D6" s="142"/>
       <c r="E6" s="60" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="141"/>
+      <c r="A7" s="138"/>
       <c r="B7" s="55" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="146"/>
+      <c r="D7" s="143"/>
       <c r="E7" s="52" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="142"/>
+      <c r="A8" s="139"/>
       <c r="B8" s="27" t="s">
         <v>34</v>
       </c>
@@ -4113,7 +4276,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="143" t="s">
+      <c r="A9" s="140" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="27" t="s">
@@ -4130,7 +4293,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="144"/>
+      <c r="A10" s="141"/>
       <c r="B10" s="56" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Se agregan prieros tres CU del mmódulo de citas.
</commit_message>
<xml_diff>
--- a/Documentacion Tecnica/PlaneacionCU/Planeacion.xlsx
+++ b/Documentacion Tecnica/PlaneacionCU/Planeacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8.1\Desktop\ESCOMobile TT2\ESCOMobile\Documentacion Tecnica\PlaneacionCU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB57B37C-B895-4D4C-9333-E670A7DDBD2F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DF0F57-000E-47BA-9412-2D23091D90FA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{6BEE2BBB-66B6-49FE-B5FF-8E26273E1384}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="130">
   <si>
     <t>Módulo</t>
   </si>
@@ -419,6 +419,9 @@
   </si>
   <si>
     <t>EM-Citas-CU1.4.1</t>
+  </si>
+  <si>
+    <t>Cancelar Cita Agendada</t>
   </si>
 </sst>
 </file>
@@ -1805,173 +1808,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="76" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1994,6 +1832,111 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="80" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="81" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2002,6 +1945,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="83" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2319,8 +2322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9913E36-BDE9-470A-AFF3-2C8FCCD03D79}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2336,15 +2339,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2370,10 +2373,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="95">
+      <c r="B3" s="109">
         <v>6</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -2393,8 +2396,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="98"/>
-      <c r="B4" s="100"/>
+      <c r="A4" s="120"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
@@ -2412,8 +2415,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="98"/>
-      <c r="B5" s="100"/>
+      <c r="A5" s="120"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
@@ -2431,8 +2434,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="98"/>
-      <c r="B6" s="100"/>
+      <c r="A6" s="120"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
@@ -2450,8 +2453,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="98"/>
-      <c r="B7" s="100"/>
+      <c r="A7" s="120"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="27" t="s">
         <v>11</v>
       </c>
@@ -2469,8 +2472,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="99"/>
-      <c r="B8" s="96"/>
+      <c r="A8" s="121"/>
+      <c r="B8" s="110"/>
       <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
@@ -2489,10 +2492,10 @@
       <c r="H8" s="91"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="95">
+      <c r="B9" s="109">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2512,8 +2515,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="94"/>
-      <c r="B10" s="96"/>
+      <c r="A10" s="105"/>
+      <c r="B10" s="110"/>
       <c r="C10" s="18" t="s">
         <v>24</v>
       </c>
@@ -2531,10 +2534,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="95">
+      <c r="B11" s="109">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2554,8 +2557,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="94"/>
-      <c r="B12" s="96"/>
+      <c r="A12" s="105"/>
+      <c r="B12" s="110"/>
       <c r="C12" s="18" t="s">
         <v>104</v>
       </c>
@@ -2573,10 +2576,10 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="103" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="95">
+      <c r="B13" s="109">
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2596,8 +2599,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="94"/>
-      <c r="B14" s="96"/>
+      <c r="A14" s="105"/>
+      <c r="B14" s="110"/>
       <c r="C14" s="18" t="s">
         <v>80</v>
       </c>
@@ -2615,10 +2618,10 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="95">
+      <c r="B15" s="109">
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2638,8 +2641,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="98"/>
-      <c r="B16" s="100"/>
+      <c r="A16" s="120"/>
+      <c r="B16" s="117"/>
       <c r="C16" s="12" t="s">
         <v>30</v>
       </c>
@@ -2657,8 +2660,8 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="98"/>
-      <c r="B17" s="100"/>
+      <c r="A17" s="120"/>
+      <c r="B17" s="117"/>
       <c r="C17" s="3" t="s">
         <v>32</v>
       </c>
@@ -2676,8 +2679,8 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="98"/>
-      <c r="B18" s="100"/>
+      <c r="A18" s="120"/>
+      <c r="B18" s="117"/>
       <c r="C18" s="12" t="s">
         <v>34</v>
       </c>
@@ -2695,8 +2698,8 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="98"/>
-      <c r="B19" s="100"/>
+      <c r="A19" s="120"/>
+      <c r="B19" s="117"/>
       <c r="C19" s="26" t="s">
         <v>36</v>
       </c>
@@ -2714,8 +2717,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="98"/>
-      <c r="B20" s="100"/>
+      <c r="A20" s="120"/>
+      <c r="B20" s="117"/>
       <c r="C20" s="3" t="s">
         <v>101</v>
       </c>
@@ -2733,8 +2736,8 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="99"/>
-      <c r="B21" s="96"/>
+      <c r="A21" s="121"/>
+      <c r="B21" s="110"/>
       <c r="C21" s="12" t="s">
         <v>38</v>
       </c>
@@ -2752,10 +2755,10 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="106" t="s">
+      <c r="A22" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="103">
+      <c r="B22" s="106">
         <v>6</v>
       </c>
       <c r="C22" s="15" t="s">
@@ -2775,8 +2778,8 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="107"/>
-      <c r="B23" s="104"/>
+      <c r="A23" s="112"/>
+      <c r="B23" s="107"/>
       <c r="C23" s="3" t="s">
         <v>97</v>
       </c>
@@ -2798,8 +2801,8 @@
       <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="107"/>
-      <c r="B24" s="104"/>
+      <c r="A24" s="112"/>
+      <c r="B24" s="107"/>
       <c r="C24" s="12" t="s">
         <v>98</v>
       </c>
@@ -2821,8 +2824,8 @@
       <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="107"/>
-      <c r="B25" s="104"/>
+      <c r="A25" s="112"/>
+      <c r="B25" s="107"/>
       <c r="C25" s="27" t="s">
         <v>102</v>
       </c>
@@ -2844,8 +2847,8 @@
       <c r="K25" s="24"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="107"/>
-      <c r="B26" s="104"/>
+      <c r="A26" s="112"/>
+      <c r="B26" s="107"/>
       <c r="C26" s="3" t="s">
         <v>99</v>
       </c>
@@ -2863,8 +2866,8 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="108"/>
-      <c r="B27" s="105"/>
+      <c r="A27" s="113"/>
+      <c r="B27" s="108"/>
       <c r="C27" s="18" t="s">
         <v>46</v>
       </c>
@@ -2882,10 +2885,10 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="145" t="s">
+      <c r="A28" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="95">
+      <c r="B28" s="109">
         <v>11</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -2905,13 +2908,13 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="146"/>
-      <c r="B29" s="100"/>
+      <c r="A29" s="115"/>
+      <c r="B29" s="117"/>
       <c r="C29" s="12" t="s">
         <v>53</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>19</v>
@@ -2924,8 +2927,8 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="146"/>
-      <c r="B30" s="100"/>
+      <c r="A30" s="115"/>
+      <c r="B30" s="117"/>
       <c r="C30" s="3" t="s">
         <v>55</v>
       </c>
@@ -2943,8 +2946,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="146"/>
-      <c r="B31" s="100"/>
+      <c r="A31" s="115"/>
+      <c r="B31" s="117"/>
       <c r="C31" s="12" t="s">
         <v>57</v>
       </c>
@@ -2962,8 +2965,8 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="146"/>
-      <c r="B32" s="100"/>
+      <c r="A32" s="115"/>
+      <c r="B32" s="117"/>
       <c r="C32" s="3" t="s">
         <v>59</v>
       </c>
@@ -2981,8 +2984,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="146"/>
-      <c r="B33" s="100"/>
+      <c r="A33" s="115"/>
+      <c r="B33" s="117"/>
       <c r="C33" s="12" t="s">
         <v>61</v>
       </c>
@@ -3000,8 +3003,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="146"/>
-      <c r="B34" s="100"/>
+      <c r="A34" s="115"/>
+      <c r="B34" s="117"/>
       <c r="C34" s="3" t="s">
         <v>63</v>
       </c>
@@ -3019,65 +3022,65 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="146"/>
-      <c r="B35" s="100"/>
+      <c r="A35" s="115"/>
+      <c r="B35" s="117"/>
       <c r="C35" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="149" t="s">
+      <c r="D35" s="94" t="s">
         <v>126</v>
       </c>
-      <c r="E35" s="150" t="s">
+      <c r="E35" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="151" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="144" t="s">
+      <c r="F35" s="96" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="93" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="146"/>
-      <c r="B36" s="148"/>
-      <c r="C36" s="153" t="s">
+      <c r="A36" s="115"/>
+      <c r="B36" s="118"/>
+      <c r="C36" s="98" t="s">
         <v>128</v>
       </c>
-      <c r="D36" s="154" t="s">
+      <c r="D36" s="99" t="s">
         <v>127</v>
       </c>
-      <c r="E36" s="155" t="s">
+      <c r="E36" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="156" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="157" t="s">
+      <c r="F36" s="101" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="102" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="146"/>
-      <c r="B37" s="148"/>
-      <c r="C37" s="153" t="s">
+      <c r="A37" s="115"/>
+      <c r="B37" s="118"/>
+      <c r="C37" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="D37" s="154" t="s">
+      <c r="D37" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="E37" s="155" t="s">
+      <c r="E37" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="156" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="157" t="s">
+      <c r="F37" s="101" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="102" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="147"/>
-      <c r="B38" s="96"/>
+      <c r="A38" s="116"/>
+      <c r="B38" s="110"/>
       <c r="C38" s="5" t="s">
         <v>67</v>
       </c>
@@ -3090,15 +3093,15 @@
       <c r="F38" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="152" t="s">
+      <c r="G38" s="97" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="93" t="s">
+      <c r="A39" s="103" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="103">
+      <c r="B39" s="106">
         <v>10</v>
       </c>
       <c r="C39" s="15" t="s">
@@ -3118,8 +3121,8 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="102"/>
-      <c r="B40" s="104"/>
+      <c r="A40" s="104"/>
+      <c r="B40" s="107"/>
       <c r="C40" s="3" t="s">
         <v>79</v>
       </c>
@@ -3137,8 +3140,8 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="102"/>
-      <c r="B41" s="104"/>
+      <c r="A41" s="104"/>
+      <c r="B41" s="107"/>
       <c r="C41" s="12" t="s">
         <v>81</v>
       </c>
@@ -3156,8 +3159,8 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="102"/>
-      <c r="B42" s="104"/>
+      <c r="A42" s="104"/>
+      <c r="B42" s="107"/>
       <c r="C42" s="3" t="s">
         <v>83</v>
       </c>
@@ -3175,8 +3178,8 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="102"/>
-      <c r="B43" s="104"/>
+      <c r="A43" s="104"/>
+      <c r="B43" s="107"/>
       <c r="C43" s="12" t="s">
         <v>77</v>
       </c>
@@ -3194,8 +3197,8 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="102"/>
-      <c r="B44" s="104"/>
+      <c r="A44" s="104"/>
+      <c r="B44" s="107"/>
       <c r="C44" s="3" t="s">
         <v>86</v>
       </c>
@@ -3213,8 +3216,8 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="102"/>
-      <c r="B45" s="104"/>
+      <c r="A45" s="104"/>
+      <c r="B45" s="107"/>
       <c r="C45" s="12" t="s">
         <v>88</v>
       </c>
@@ -3232,8 +3235,8 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="102"/>
-      <c r="B46" s="104"/>
+      <c r="A46" s="104"/>
+      <c r="B46" s="107"/>
       <c r="C46" s="3" t="s">
         <v>90</v>
       </c>
@@ -3251,8 +3254,8 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="102"/>
-      <c r="B47" s="104"/>
+      <c r="A47" s="104"/>
+      <c r="B47" s="107"/>
       <c r="C47" s="12" t="s">
         <v>92</v>
       </c>
@@ -3270,8 +3273,8 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="94"/>
-      <c r="B48" s="105"/>
+      <c r="A48" s="105"/>
+      <c r="B48" s="108"/>
       <c r="C48" s="5" t="s">
         <v>94</v>
       </c>
@@ -3290,6 +3293,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="A39:A48"/>
     <mergeCell ref="B39:B48"/>
     <mergeCell ref="A13:A14"/>
@@ -3302,11 +3310,6 @@
     <mergeCell ref="B28:B38"/>
     <mergeCell ref="A15:A21"/>
     <mergeCell ref="B15:B21"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3332,14 +3335,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="144" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
@@ -3362,10 +3365,10 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="158" t="s">
+      <c r="A3" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="110">
+      <c r="B3" s="135">
         <v>20</v>
       </c>
       <c r="C3" s="34" t="s">
@@ -3374,7 +3377,7 @@
       <c r="D3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="121" t="s">
+      <c r="E3" s="151" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="36" t="s">
@@ -3382,29 +3385,29 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="159"/>
-      <c r="B4" s="111"/>
+      <c r="A4" s="139"/>
+      <c r="B4" s="136"/>
       <c r="C4" s="30" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="122"/>
+      <c r="E4" s="134"/>
       <c r="F4" s="36" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="159"/>
-      <c r="B5" s="111"/>
+      <c r="A5" s="139"/>
+      <c r="B5" s="136"/>
       <c r="C5" s="30" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="123" t="s">
+      <c r="E5" s="132" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="36" t="s">
@@ -3412,29 +3415,29 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="159"/>
-      <c r="B6" s="111"/>
+      <c r="A6" s="139"/>
+      <c r="B6" s="136"/>
       <c r="C6" s="30" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="122"/>
+      <c r="E6" s="134"/>
       <c r="F6" s="36" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="159"/>
-      <c r="B7" s="111"/>
+      <c r="A7" s="139"/>
+      <c r="B7" s="136"/>
       <c r="C7" s="30" t="s">
         <v>71</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="123" t="s">
+      <c r="E7" s="132" t="s">
         <v>70</v>
       </c>
       <c r="F7" s="36" t="s">
@@ -3446,15 +3449,15 @@
       <c r="K7" s="24"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="159"/>
-      <c r="B8" s="111"/>
+      <c r="A8" s="139"/>
+      <c r="B8" s="136"/>
       <c r="C8" s="30" t="s">
         <v>80</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="122"/>
+      <c r="E8" s="134"/>
       <c r="F8" s="36" t="s">
         <v>10</v>
       </c>
@@ -3464,15 +3467,15 @@
       <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="159"/>
-      <c r="B9" s="111"/>
+      <c r="A9" s="139"/>
+      <c r="B9" s="136"/>
       <c r="C9" s="30" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="123" t="s">
+      <c r="E9" s="132" t="s">
         <v>27</v>
       </c>
       <c r="F9" s="36" t="s">
@@ -3484,15 +3487,15 @@
       <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="159"/>
-      <c r="B10" s="111"/>
+      <c r="A10" s="139"/>
+      <c r="B10" s="136"/>
       <c r="C10" s="30" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="124"/>
+      <c r="E10" s="133"/>
       <c r="F10" s="36" t="s">
         <v>16</v>
       </c>
@@ -3502,15 +3505,15 @@
       <c r="K10" s="24"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="159"/>
-      <c r="B11" s="111"/>
+      <c r="A11" s="139"/>
+      <c r="B11" s="136"/>
       <c r="C11" s="30" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="124"/>
+      <c r="E11" s="133"/>
       <c r="F11" s="36" t="s">
         <v>10</v>
       </c>
@@ -3520,15 +3523,15 @@
       <c r="K11" s="24"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="159"/>
-      <c r="B12" s="111"/>
+      <c r="A12" s="139"/>
+      <c r="B12" s="136"/>
       <c r="C12" s="30" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="124"/>
+      <c r="E12" s="133"/>
       <c r="F12" s="37" t="s">
         <v>16</v>
       </c>
@@ -3538,15 +3541,15 @@
       <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="159"/>
-      <c r="B13" s="111"/>
+      <c r="A13" s="139"/>
+      <c r="B13" s="136"/>
       <c r="C13" s="30" t="s">
         <v>101</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="124"/>
+      <c r="E13" s="133"/>
       <c r="F13" s="36" t="s">
         <v>10</v>
       </c>
@@ -3556,15 +3559,15 @@
       <c r="K13" s="24"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="159"/>
-      <c r="B14" s="111"/>
+      <c r="A14" s="139"/>
+      <c r="B14" s="136"/>
       <c r="C14" s="30" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="122"/>
+      <c r="E14" s="134"/>
       <c r="F14" s="36" t="s">
         <v>10</v>
       </c>
@@ -3574,15 +3577,15 @@
       <c r="K14" s="24"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="159"/>
-      <c r="B15" s="111"/>
+      <c r="A15" s="139"/>
+      <c r="B15" s="136"/>
       <c r="C15" s="30" t="s">
         <v>51</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="123" t="s">
+      <c r="E15" s="132" t="s">
         <v>69</v>
       </c>
       <c r="F15" s="37" t="s">
@@ -3594,15 +3597,15 @@
       <c r="K15" s="24"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="159"/>
-      <c r="B16" s="111"/>
+      <c r="A16" s="139"/>
+      <c r="B16" s="136"/>
       <c r="C16" s="30" t="s">
         <v>55</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="124"/>
+      <c r="E16" s="133"/>
       <c r="F16" s="37" t="s">
         <v>16</v>
       </c>
@@ -3612,15 +3615,15 @@
       <c r="K16" s="24"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="159"/>
-      <c r="B17" s="111"/>
+      <c r="A17" s="139"/>
+      <c r="B17" s="136"/>
       <c r="C17" s="30" t="s">
         <v>65</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="122"/>
+      <c r="E17" s="134"/>
       <c r="F17" s="37" t="s">
         <v>16</v>
       </c>
@@ -3630,15 +3633,15 @@
       <c r="K17" s="24"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="159"/>
-      <c r="B18" s="111"/>
+      <c r="A18" s="139"/>
+      <c r="B18" s="136"/>
       <c r="C18" s="30" t="s">
         <v>75</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="123" t="s">
+      <c r="E18" s="132" t="s">
         <v>74</v>
       </c>
       <c r="F18" s="36" t="s">
@@ -3650,15 +3653,15 @@
       <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="159"/>
-      <c r="B19" s="111"/>
+      <c r="A19" s="139"/>
+      <c r="B19" s="136"/>
       <c r="C19" s="30" t="s">
         <v>79</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="124"/>
+      <c r="E19" s="133"/>
       <c r="F19" s="36" t="s">
         <v>10</v>
       </c>
@@ -3668,15 +3671,15 @@
       <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="159"/>
-      <c r="B20" s="111"/>
+      <c r="A20" s="139"/>
+      <c r="B20" s="136"/>
       <c r="C20" s="30" t="s">
         <v>86</v>
       </c>
       <c r="D20" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="124"/>
+      <c r="E20" s="133"/>
       <c r="F20" s="48" t="s">
         <v>10</v>
       </c>
@@ -3686,15 +3689,15 @@
       <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="159"/>
-      <c r="B21" s="111"/>
+      <c r="A21" s="139"/>
+      <c r="B21" s="136"/>
       <c r="C21" s="30" t="s">
         <v>88</v>
       </c>
       <c r="D21" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="124"/>
+      <c r="E21" s="133"/>
       <c r="F21" s="36" t="s">
         <v>10</v>
       </c>
@@ -3704,15 +3707,15 @@
       <c r="K21" s="24"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="160"/>
-      <c r="B22" s="112"/>
+      <c r="A22" s="140"/>
+      <c r="B22" s="137"/>
       <c r="C22" s="38" t="s">
         <v>90</v>
       </c>
       <c r="D22" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="125"/>
+      <c r="E22" s="152"/>
       <c r="F22" s="40" t="s">
         <v>10</v>
       </c>
@@ -3722,10 +3725,10 @@
       <c r="K22" s="24"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="116" t="s">
+      <c r="A23" s="148" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="113">
+      <c r="B23" s="145">
         <v>23</v>
       </c>
       <c r="C23" s="41" t="s">
@@ -3746,15 +3749,15 @@
       <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="117"/>
-      <c r="B24" s="114"/>
+      <c r="A24" s="149"/>
+      <c r="B24" s="146"/>
       <c r="C24" s="32" t="s">
         <v>43</v>
       </c>
       <c r="D24" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="119" t="s">
+      <c r="E24" s="141" t="s">
         <v>42</v>
       </c>
       <c r="F24" s="43" t="s">
@@ -3766,15 +3769,15 @@
       <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="117"/>
-      <c r="B25" s="114"/>
+      <c r="A25" s="149"/>
+      <c r="B25" s="146"/>
       <c r="C25" s="32" t="s">
         <v>104</v>
       </c>
       <c r="D25" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="E25" s="126"/>
+      <c r="E25" s="143"/>
       <c r="F25" s="43" t="s">
         <v>16</v>
       </c>
@@ -3784,8 +3787,8 @@
       <c r="K25" s="24"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="117"/>
-      <c r="B26" s="114"/>
+      <c r="A26" s="149"/>
+      <c r="B26" s="146"/>
       <c r="C26" s="32" t="s">
         <v>34</v>
       </c>
@@ -3800,15 +3803,15 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="117"/>
-      <c r="B27" s="114"/>
+      <c r="A27" s="149"/>
+      <c r="B27" s="146"/>
       <c r="C27" s="32" t="s">
         <v>44</v>
       </c>
       <c r="D27" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="119" t="s">
+      <c r="E27" s="141" t="s">
         <v>108</v>
       </c>
       <c r="F27" s="43" t="s">
@@ -3816,85 +3819,85 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="117"/>
-      <c r="B28" s="114"/>
+      <c r="A28" s="149"/>
+      <c r="B28" s="146"/>
       <c r="C28" s="32" t="s">
         <v>97</v>
       </c>
       <c r="D28" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="120"/>
+      <c r="E28" s="142"/>
       <c r="F28" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="117"/>
-      <c r="B29" s="114"/>
+      <c r="A29" s="149"/>
+      <c r="B29" s="146"/>
       <c r="C29" s="32" t="s">
         <v>98</v>
       </c>
       <c r="D29" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="120"/>
+      <c r="E29" s="142"/>
       <c r="F29" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="117"/>
-      <c r="B30" s="114"/>
+      <c r="A30" s="149"/>
+      <c r="B30" s="146"/>
       <c r="C30" s="32" t="s">
         <v>102</v>
       </c>
       <c r="D30" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="E30" s="120"/>
+      <c r="E30" s="142"/>
       <c r="F30" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="117"/>
-      <c r="B31" s="114"/>
+      <c r="A31" s="149"/>
+      <c r="B31" s="146"/>
       <c r="C31" s="32" t="s">
         <v>99</v>
       </c>
       <c r="D31" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="120"/>
+      <c r="E31" s="142"/>
       <c r="F31" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="117"/>
-      <c r="B32" s="114"/>
+      <c r="A32" s="149"/>
+      <c r="B32" s="146"/>
       <c r="C32" s="32" t="s">
         <v>46</v>
       </c>
       <c r="D32" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="126"/>
+      <c r="E32" s="143"/>
       <c r="F32" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="117"/>
-      <c r="B33" s="114"/>
+      <c r="A33" s="149"/>
+      <c r="B33" s="146"/>
       <c r="C33" s="32" t="s">
         <v>53</v>
       </c>
       <c r="D33" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="119" t="s">
+      <c r="E33" s="141" t="s">
         <v>69</v>
       </c>
       <c r="F33" s="43" t="s">
@@ -3902,113 +3905,113 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="117"/>
-      <c r="B34" s="114"/>
+      <c r="A34" s="149"/>
+      <c r="B34" s="146"/>
       <c r="C34" s="32" t="s">
         <v>57</v>
       </c>
       <c r="D34" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="120"/>
+      <c r="E34" s="142"/>
       <c r="F34" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="117"/>
-      <c r="B35" s="114"/>
+      <c r="A35" s="149"/>
+      <c r="B35" s="146"/>
       <c r="C35" s="32" t="s">
         <v>59</v>
       </c>
       <c r="D35" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="120"/>
+      <c r="E35" s="142"/>
       <c r="F35" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="117"/>
-      <c r="B36" s="114"/>
+      <c r="A36" s="149"/>
+      <c r="B36" s="146"/>
       <c r="C36" s="32" t="s">
         <v>61</v>
       </c>
       <c r="D36" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="E36" s="120"/>
+      <c r="E36" s="142"/>
       <c r="F36" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="117"/>
-      <c r="B37" s="114"/>
+      <c r="A37" s="149"/>
+      <c r="B37" s="146"/>
       <c r="C37" s="32" t="s">
         <v>63</v>
       </c>
       <c r="D37" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="E37" s="120"/>
+      <c r="E37" s="142"/>
       <c r="F37" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="117"/>
-      <c r="B38" s="114"/>
+      <c r="A38" s="149"/>
+      <c r="B38" s="146"/>
       <c r="C38" s="32" t="s">
         <v>125</v>
       </c>
       <c r="D38" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="E38" s="120"/>
+      <c r="E38" s="142"/>
       <c r="F38" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="117"/>
-      <c r="B39" s="114"/>
+      <c r="A39" s="149"/>
+      <c r="B39" s="146"/>
       <c r="C39" s="32" t="s">
         <v>128</v>
       </c>
       <c r="D39" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="E39" s="120"/>
+      <c r="E39" s="142"/>
       <c r="F39" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="117"/>
-      <c r="B40" s="114"/>
+      <c r="A40" s="149"/>
+      <c r="B40" s="146"/>
       <c r="C40" s="32" t="s">
         <v>67</v>
       </c>
       <c r="D40" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="E40" s="126"/>
+      <c r="E40" s="143"/>
       <c r="F40" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="117"/>
-      <c r="B41" s="114"/>
+      <c r="A41" s="149"/>
+      <c r="B41" s="146"/>
       <c r="C41" s="32" t="s">
         <v>81</v>
       </c>
       <c r="D41" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="E41" s="119" t="s">
+      <c r="E41" s="141" t="s">
         <v>74</v>
       </c>
       <c r="F41" s="43" t="s">
@@ -4018,67 +4021,67 @@
       <c r="H41" s="24"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="117"/>
-      <c r="B42" s="114"/>
+      <c r="A42" s="149"/>
+      <c r="B42" s="146"/>
       <c r="C42" s="32" t="s">
         <v>83</v>
       </c>
       <c r="D42" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="E42" s="120"/>
+      <c r="E42" s="142"/>
       <c r="F42" s="43" t="s">
         <v>10</v>
       </c>
       <c r="G42" s="45"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="117"/>
-      <c r="B43" s="114"/>
+      <c r="A43" s="149"/>
+      <c r="B43" s="146"/>
       <c r="C43" s="32" t="s">
         <v>77</v>
       </c>
       <c r="D43" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="E43" s="120"/>
+      <c r="E43" s="142"/>
       <c r="F43" s="44" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="117"/>
-      <c r="B44" s="114"/>
+      <c r="A44" s="149"/>
+      <c r="B44" s="146"/>
       <c r="C44" s="32" t="s">
         <v>92</v>
       </c>
       <c r="D44" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="E44" s="120"/>
+      <c r="E44" s="142"/>
       <c r="F44" s="43" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="118"/>
-      <c r="B45" s="115"/>
+      <c r="A45" s="150"/>
+      <c r="B45" s="147"/>
       <c r="C45" s="66" t="s">
         <v>94</v>
       </c>
       <c r="D45" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="E45" s="120"/>
+      <c r="E45" s="142"/>
       <c r="F45" s="68" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="127" t="s">
+      <c r="A46" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="130">
+      <c r="B46" s="126">
         <v>2</v>
       </c>
       <c r="C46" s="69" t="s">
@@ -4087,7 +4090,7 @@
       <c r="D46" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="E46" s="133" t="s">
+      <c r="E46" s="129" t="s">
         <v>21</v>
       </c>
       <c r="F46" s="71" t="s">
@@ -4095,42 +4098,35 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="128"/>
-      <c r="B47" s="131"/>
+      <c r="A47" s="124"/>
+      <c r="B47" s="127"/>
       <c r="C47" s="64" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="E47" s="134"/>
+      <c r="E47" s="130"/>
       <c r="F47" s="72" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="129"/>
-      <c r="B48" s="132"/>
+      <c r="A48" s="125"/>
+      <c r="B48" s="128"/>
       <c r="C48" s="73" t="s">
         <v>13</v>
       </c>
       <c r="D48" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="E48" s="135"/>
+      <c r="E48" s="131"/>
       <c r="F48" s="75" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="B3:B22"/>
-    <mergeCell ref="A3:A22"/>
-    <mergeCell ref="E33:E40"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B23:B45"/>
     <mergeCell ref="A23:A45"/>
@@ -4142,6 +4138,13 @@
     <mergeCell ref="E27:E32"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="E5:E6"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="B3:B22"/>
+    <mergeCell ref="A3:A22"/>
+    <mergeCell ref="E33:E40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4166,13 +4169,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="153" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
@@ -4192,7 +4195,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="154" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="54" t="s">
@@ -4201,7 +4204,7 @@
       <c r="C3" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="142" t="s">
+      <c r="D3" s="159" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="62" t="s">
@@ -4209,59 +4212,59 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="138"/>
+      <c r="A4" s="155"/>
       <c r="B4" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="142"/>
+      <c r="D4" s="159"/>
       <c r="E4" s="61" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="138"/>
+      <c r="A5" s="155"/>
       <c r="B5" s="55" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="142"/>
+      <c r="D5" s="159"/>
       <c r="E5" s="60" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="138"/>
+      <c r="A6" s="155"/>
       <c r="B6" s="27" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="142"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="60" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="138"/>
+      <c r="A7" s="155"/>
       <c r="B7" s="55" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="143"/>
+      <c r="D7" s="160"/>
       <c r="E7" s="52" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="139"/>
+      <c r="A8" s="156"/>
       <c r="B8" s="27" t="s">
         <v>34</v>
       </c>
@@ -4276,7 +4279,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="140" t="s">
+      <c r="A9" s="157" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="27" t="s">
@@ -4293,7 +4296,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="141"/>
+      <c r="A10" s="158"/>
       <c r="B10" s="56" t="s">
         <v>17</v>
       </c>

</xml_diff>